<commit_message>
updates to defaults.xls and the python script for making the ICD
</commit_message>
<xml_diff>
--- a/SimCADO/simcado/docs/SimCADO_defaults.xlsx
+++ b/SimCADO/simcado/docs/SimCADO_defaults.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Tabelle2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="206">
   <si>
     <t xml:space="preserve">Section</t>
   </si>
@@ -67,81 +68,72 @@
     <t xml:space="preserve">Responsible_WP</t>
   </si>
   <si>
-    <t xml:space="preserve">MICADO optical elements</t>
+    <t xml:space="preserve">MICADO Spatial effects</t>
   </si>
   <si>
     <t xml:space="preserve">Point spread function</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCOPE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCOPE_PSF_FILE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data/PSF_POPPY.fits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Generated by JWST/POPPY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02.11.2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n</t>
   </si>
   <si>
     <t xml:space="preserve">Currently waiting on SCAO PSFs for the default. If there are none ready, we will ship with the ESO LTAO PSFs from the 2012 AO study for a 42m mirror. 
 Other options include using the POPPY PSF simulator from the JWST to make PSFs on the fly</t>
   </si>
   <si>
+    <t xml:space="preserve">SCOPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCOPE_PSF_FILE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data/PSF_LTAO.fits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESO E-ELT optics webpage (2012 study)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02.11.2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">im</t>
+  </si>
+  <si>
     <t xml:space="preserve">Atmospheric Dispersion Correction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INST_ADC_PERFORMANCE </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Best guess</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REAL DATA NEEDED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INST_ADC_NUM_SURFACES </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email from Ric</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source needed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INST_ADC_TC </t>
-  </si>
-  <si>
-    <t xml:space="preserve">data/TC_ADC.dat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">y</t>
   </si>
   <si>
     <t xml:space="preserve">The number of surfaces in the ADC is set to 8. A constant transmission curve of 0.98 is assumed for each of these surfaces, thus the total throughput of a perfectly functioning ADC is `0.98^8 = 0.85` over the wavelength range 0.5-3.0um
 SimCADO implements an inverse ADC. It assumes that the ADC corrects perfectly for the dispersion induced by the atmosphere. If the ADC isn't working as it should, i.e. `INST_ADC_PERFORMANCE` less than 100%, SimCADO calculates the distance an uncorrected image/slice would be from the centre of the FoV, then shifts the image/slice by `shift = AD * (1 - 0.01 * INST_ADC_PERFORMANCE)`. By calculating this shift for each slice in the spectral cube, SimCADO recreates the smearing effect of an imperfect ADC</t>
   </si>
   <si>
+    <t xml:space="preserve">INST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INST_ADC_PERFORMANCE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Best guess</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REAL DATA NEEDED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INST_ADC_NUM_SURFACES </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email from Ric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source needed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INST_ADC_TC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">data/TC_ADC.dat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y</t>
+  </si>
+  <si>
     <t xml:space="preserve">Derotator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INST_DEROT_PERFORMANCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INST_DEROT_PROFILE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">linear</t>
   </si>
   <si>
     <t xml:space="preserve">**Not fully implemented**
@@ -149,32 +141,38 @@
 `INST_DEROT_PROFILE` can be linear or gaussian</t>
   </si>
   <si>
+    <t xml:space="preserve">INST_DEROT_PERFORMANCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INST_DEROT_PROFILE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">linear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MICADO transmission effects</t>
+  </si>
+  <si>
     <t xml:space="preserve">MICADO mirrors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INST_NUM_MIRRORS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INST_MIRROR_TC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data/TC_mirror_mgf2agal.dat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESO E-ELT technical database</t>
   </si>
   <si>
     <t xml:space="preserve">For Wide-field (4mas) mode, 11 mirrors are in the optical train. For Zoom (1.5mas) mode, 13 mirrors are used. 
 The default mirror coating is currently the same as the E-ELTs MgF2 coating with a AgAl protective layer. **Are MICADOs mirror coatings similar?**</t>
   </si>
   <si>
+    <t xml:space="preserve">INST_NUM_MIRRORS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INST_MIRROR_TC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data/TC_mirror_mgf2agal.dat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESO E-ELT technical database</t>
+  </si>
+  <si>
     <t xml:space="preserve">Filters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INST_FILTER_TC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data/TC_filter_K.dat</t>
   </si>
   <si>
     <t xml:space="preserve">The transmission curves for filters are for the filter as a whole unit. Individual surface transmission curves (i.e. 2 per filter) are not taken into account.
@@ -191,6 +189,12 @@
 More filters can be added upon request</t>
   </si>
   <si>
+    <t xml:space="preserve">INST_FILTER_TC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data/TC_filter_Ks.dat</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cryostat window</t>
   </si>
   <si>
@@ -218,6 +222,9 @@
     <t xml:space="preserve">Dichroics</t>
   </si>
   <si>
+    <t xml:space="preserve">The question is if these are really necessary in the simulations, seeing as they only affect a small area of the pupil</t>
+  </si>
+  <si>
     <t xml:space="preserve">INST_DICHROIC_NUM_SURFACES</t>
   </si>
   <si>
@@ -227,12 +234,12 @@
     <t xml:space="preserve">data/TC_dichroic.dat</t>
   </si>
   <si>
-    <t xml:space="preserve">The question is if these are really necessary in the simulations, seeing as they only affect a small area of the pupil</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pupil optics</t>
   </si>
   <si>
+    <t xml:space="preserve">**How do the pupil optics affect the image in practical terms?**</t>
+  </si>
+  <si>
     <t xml:space="preserve">INST_PUPIL_NUM_SURFACES</t>
   </si>
   <si>
@@ -242,9 +249,6 @@
     <t xml:space="preserve">data/TC_pupil.dat</t>
   </si>
   <si>
-    <t xml:space="preserve">**How do the pupil optics affect the image in practical terms?**</t>
-  </si>
-  <si>
     <t xml:space="preserve">MICADO Detector effects</t>
   </si>
   <si>
@@ -261,33 +265,6 @@
   </si>
   <si>
     <t xml:space="preserve">Chip noise characteristics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FPA_USE_NOISE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FPA_NOISE_PATH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data/FPA_noise.fits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FPA_READOUT_MEDIAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FPA_READOUT_STDEV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FPA_DARK_MEDIAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FPA_DARK_STDEV</t>
   </si>
   <si>
     <t xml:space="preserve">If a noise file (`FPA_NOISE_PATH`) is provided, then this is used as the chip noise. This file must however be downloaded and added to the package as it is not shipped with SimCADO due to size
@@ -295,6 +272,33 @@
 Read noise and dark current are based on the defaults from the Hawaii xRG noise generator code (Rauscher 2015)</t>
   </si>
   <si>
+    <t xml:space="preserve">FPA_USE_NOISE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FPA_NOISE_PATH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data/FPA_noise.fits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FPA_READOUT_MEDIAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FPA_READOUT_STDEV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FPA_DARK_MEDIAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FPA_DARK_STDEV</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chip dynamic range</t>
   </si>
   <si>
@@ -308,48 +312,6 @@
   </si>
   <si>
     <t xml:space="preserve">Hawaii 4RG Simulator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HXRG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HXRG_NUM_OUTPUTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of read out channels per chip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HXRG_NUM_ROW_OH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of row overhead in pixels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HXRG_CORR_PINK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Factor for correlated pink noise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HXRG_UNCORR_PINK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Factor for uncorrelated pink noise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HXRG_ALT_COL_NOISE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Factor for Alternating Column Noise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HXRG_PEDESTAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Magnitude of pedestal drift</t>
   </si>
   <si>
     <r>
@@ -383,22 +345,49 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">HXRG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HXRG_NUM_OUTPUTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of read out channels per chip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HXRG_NUM_ROW_OH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of row overhead in pixels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HXRG_CORR_PINK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Factor for correlated pink noise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HXRG_UNCORR_PINK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Factor for uncorrelated pink noise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HXRG_ALT_COL_NOISE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Factor for Alternating Column Noise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HXRG_PEDESTAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnitude of pedestal drift</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pixel sensitivity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FPA_PIXEL_MAP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FPA_DEAD_PIXELS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Simms+ 2007 for H2RG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FPA_DEAD_LINES</t>
   </si>
   <si>
     <t xml:space="preserve">The pixel sensitivity of a detector. Can be specified as a FITS file covering the 4k detector, or a random sample of dead lines/pixels. The default is  `FPA_PIXEL_MAP = none`, and so SimCADO creates dead pixels and lines
@@ -406,13 +395,22 @@
 **Needs to be revised for hot pixels**</t>
   </si>
   <si>
+    <t xml:space="preserve">FPA_PIXEL_MAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FPA_DEAD_PIXELS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simms+ 2007 for H2RG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FPA_DEAD_LINES</t>
+  </si>
+  <si>
     <t xml:space="preserve">Detector layout</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FPA_CHIP_LAYOUT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data/FPA_chip_layout_small.dat</t>
   </si>
   <si>
     <t xml:space="preserve">For the sake of quick computations, the default value for the SimCADO detector array (`small`) describes a single 1024x1024 pixel windowed read-out at the centre of the FoV. 
@@ -426,6 +424,12 @@
 Custom layouts for different windowing schemes are also possible by specifying the position of the centre of the window and its width/height in pixels in `arcsec` relative to the centre of the FoV.</t>
   </si>
   <si>
+    <t xml:space="preserve">FPA_CHIP_LAYOUT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data/FPA_chip_layout_small.dat</t>
+  </si>
+  <si>
     <t xml:space="preserve">MICADO Detector read modes</t>
   </si>
   <si>
@@ -433,30 +437,33 @@
   </si>
   <si>
     <t xml:space="preserve">MAORY mirrors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INST_NUM_AO_MIRRORS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INST_MIRROR_AO_TC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INST_MIRROR_AO_SUM_AREA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.28 m^2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INST_MIRROR_AO_TEMP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0 deg Celcius</t>
   </si>
   <si>
     <t xml:space="preserve">The same mirror coating is assumed for the MAORY mirrors as for the E-ELT and MICADO
 Here we also assume 8x 1m class mirrors, held at ambient temperature emitting as grey bodies. The total surface area (`INST_MIRROR_AO_SUM_AREA`) of all mirrors in the AO system are used for the thermal background</t>
   </si>
   <si>
+    <t xml:space="preserve">INST_NUM_AO_MIRRORS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INST_MIRROR_AO_TC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INST_MIRROR_AO_SUM_AREA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.28 m^2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INST_MIRROR_AO_TEMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 deg Celcius</t>
+  </si>
+  <si>
     <t xml:space="preserve">Telescope optics</t>
   </si>
   <si>
@@ -529,12 +536,6 @@
     <t xml:space="preserve">SCOPE_M5_DIAMETER_IN</t>
   </si>
   <si>
-    <t xml:space="preserve">SCOPE_M6_DIAMETER_OUT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCOPE_M6_DIAMETER_IN</t>
-  </si>
-  <si>
     <t xml:space="preserve">Wind jitter and telescope vibrations</t>
   </si>
   <si>
@@ -571,6 +572,9 @@
     <t xml:space="preserve">data/skytable.fits</t>
   </si>
   <si>
+    <t xml:space="preserve">ec</t>
+  </si>
+  <si>
     <t xml:space="preserve">ATMO_BG_MAGNITUDE</t>
   </si>
   <si>
@@ -583,6 +587,9 @@
     <t xml:space="preserve">ATMO_TC</t>
   </si>
   <si>
+    <t xml:space="preserve">tc</t>
+  </si>
+  <si>
     <t xml:space="preserve">Atmospheric conditions</t>
   </si>
   <si>
@@ -623,6 +630,72 @@
   </si>
   <si>
     <t xml:space="preserve">EOF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List of Stellar Spectra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List of Galaxy Spectra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List of filters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OBAFGKM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pickles catalogue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ulirg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arp220</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBVRIzYJHKKs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elliptical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brown_dwarf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gl229b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">starburst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m82</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nebula</t>
+  </si>
+  <si>
+    <t xml:space="preserve">orion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quasar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spiral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interacting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ugc5101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ftp://ftp.stsci.edu/cdbs/etc/source/</t>
   </si>
 </sst>
 </file>
@@ -761,8 +834,8 @@
   </sheetPr>
   <dimension ref="A1:Z126"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H76" activeCellId="0" sqref="H76"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E89" activeCellId="0" sqref="E89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -841,33 +914,23 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="77.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="0"/>
+      <c r="D2" s="0"/>
+      <c r="E2" s="0"/>
+      <c r="F2" s="0"/>
+      <c r="G2" s="0"/>
+      <c r="H2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="J2" s="0"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -885,19 +948,29 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="77.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="0"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -915,30 +988,20 @@
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
     </row>
-    <row r="4" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="205.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="I4" s="0"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
@@ -961,23 +1024,23 @@
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -1001,27 +1064,25 @@
       <c r="A6" s="2"/>
       <c r="B6" s="0"/>
       <c r="C6" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>8</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>34</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -1039,19 +1100,31 @@
       <c r="Y6" s="2"/>
       <c r="Z6" s="2"/>
     </row>
-    <row r="7" customFormat="false" ht="205.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2" t="s">
+      <c r="C7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="0"/>
+      <c r="I7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -1069,30 +1142,20 @@
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
     </row>
-    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="141.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -1115,23 +1178,23 @@
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>39</v>
+      <c r="E9" s="2" t="n">
+        <v>100</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -1151,18 +1214,28 @@
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
     </row>
-    <row r="10" customFormat="false" ht="141.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2" t="s">
+      <c r="C10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="0"/>
+      <c r="I10" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
@@ -1181,30 +1254,22 @@
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
     </row>
-    <row r="11" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2"/>
+    <row r="11" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="B11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="2" t="n">
-        <v>11</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2" t="s">
-        <v>31</v>
-      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
@@ -1223,31 +1288,29 @@
       <c r="Y11" s="2"/>
       <c r="Z11" s="2"/>
     </row>
-    <row r="12" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="2" t="s">
         <v>44</v>
       </c>
+      <c r="E12" s="2" t="n">
+        <v>11</v>
+      </c>
       <c r="F12" s="2" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>34</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
@@ -1265,19 +1328,31 @@
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
     </row>
-    <row r="13" customFormat="false" ht="90.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2" t="s">
+      <c r="C13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
+      <c r="F13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="0"/>
+      <c r="I13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
@@ -1295,31 +1370,21 @@
       <c r="Y13" s="2"/>
       <c r="Z13" s="2"/>
     </row>
-    <row r="14" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="230.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
@@ -1337,19 +1402,29 @@
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
     </row>
-    <row r="15" customFormat="false" ht="230.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2" t="s">
+      <c r="C15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="E15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="0"/>
       <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
+      <c r="J15" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
@@ -1370,23 +1445,13 @@
     <row r="16" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -1411,25 +1476,23 @@
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>54</v>
+      <c r="E17" s="2" t="n">
+        <v>4</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-      <c r="J17" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
@@ -1447,17 +1510,29 @@
       <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
+      <c r="C18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
+      <c r="J18" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
@@ -1478,23 +1553,13 @@
     <row r="19" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -1515,14 +1580,24 @@
       <c r="Y19" s="2"/>
       <c r="Z19" s="2"/>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
+      <c r="C20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H20" s="0"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -1543,27 +1618,19 @@
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
     </row>
-    <row r="21" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="37.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E21" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H21" s="0"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
@@ -1586,24 +1653,24 @@
     <row r="22" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
+      <c r="C22" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="D22" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E22" s="2" t="s">
         <v>62</v>
       </c>
+      <c r="E22" s="2" t="n">
+        <v>2</v>
+      </c>
       <c r="F22" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H22" s="0"/>
       <c r="I22" s="2"/>
-      <c r="J22" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
@@ -1621,19 +1688,27 @@
       <c r="Y22" s="2"/>
       <c r="Z22" s="2"/>
     </row>
-    <row r="23" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="1" t="s">
+      <c r="D23" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="E23" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H23" s="0"/>
       <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
+      <c r="J23" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
@@ -1651,30 +1726,20 @@
       <c r="Y23" s="2"/>
       <c r="Z23" s="2"/>
     </row>
-    <row r="24" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E24" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H24" s="0"/>
-      <c r="I24" s="2" t="s">
-        <v>31</v>
-      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
@@ -1697,23 +1762,23 @@
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E25" s="2" t="s">
         <v>67</v>
       </c>
+      <c r="E25" s="2" t="n">
+        <v>2</v>
+      </c>
       <c r="F25" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H25" s="0"/>
       <c r="I25" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
@@ -1733,18 +1798,28 @@
       <c r="Y25" s="2"/>
       <c r="Z25" s="2"/>
     </row>
-    <row r="26" customFormat="false" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="1" t="s">
+      <c r="C26" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="I26" s="2"/>
+      <c r="E26" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H26" s="0"/>
+      <c r="I26" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
@@ -1765,29 +1840,19 @@
     </row>
     <row r="27" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C27" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>73</v>
-      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
-      <c r="I27" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
@@ -1805,17 +1870,27 @@
       <c r="Y27" s="2"/>
       <c r="Z27" s="2"/>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2"/>
       <c r="B28" s="0"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="2"/>
+      <c r="C28" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
+      <c r="I28" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
@@ -1833,23 +1908,19 @@
       <c r="Y28" s="2"/>
       <c r="Z28" s="2"/>
     </row>
-    <row r="29" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="141.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2"/>
       <c r="B29" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D29" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>76</v>
-      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
+      <c r="H29" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
@@ -1873,7 +1944,7 @@
       <c r="A30" s="2"/>
       <c r="B30" s="0"/>
       <c r="C30" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>77</v>
@@ -1907,13 +1978,13 @@
       <c r="A31" s="2"/>
       <c r="B31" s="0"/>
       <c r="C31" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D31" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E31" s="2" t="n">
-        <v>4</v>
+      <c r="E31" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
@@ -1941,13 +2012,13 @@
       <c r="A32" s="2"/>
       <c r="B32" s="0"/>
       <c r="C32" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
@@ -1975,13 +2046,13 @@
       <c r="A33" s="2"/>
       <c r="B33" s="0"/>
       <c r="C33" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E33" s="2" t="s">
         <v>82</v>
+      </c>
+      <c r="E33" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
@@ -2009,13 +2080,13 @@
       <c r="A34" s="2"/>
       <c r="B34" s="0"/>
       <c r="C34" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>83</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
@@ -2039,17 +2110,21 @@
       <c r="Y34" s="2"/>
       <c r="Z34" s="2"/>
     </row>
-    <row r="35" customFormat="false" ht="141.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2"/>
       <c r="B35" s="0"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
+      <c r="C35" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
-      <c r="H35" s="2" t="s">
-        <v>84</v>
-      </c>
+      <c r="H35" s="0"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
@@ -2069,18 +2144,14 @@
       <c r="Y35" s="2"/>
       <c r="Z35" s="2"/>
     </row>
-    <row r="36" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2"/>
       <c r="B36" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C36" s="2"/>
-      <c r="D36" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E36" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
@@ -2103,15 +2174,15 @@
       <c r="Y36" s="2"/>
       <c r="Z36" s="2"/>
     </row>
-    <row r="37" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2"/>
       <c r="B37" s="0"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E37" s="4" t="n">
-        <v>100000</v>
+      <c r="E37" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
@@ -2135,15 +2206,15 @@
       <c r="Y37" s="2"/>
       <c r="Z37" s="2"/>
     </row>
-    <row r="38" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2"/>
       <c r="B38" s="0"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>57</v>
+      <c r="E38" s="4" t="n">
+        <v>100000</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
@@ -2167,12 +2238,16 @@
       <c r="Y38" s="2"/>
       <c r="Z38" s="2"/>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2"/>
       <c r="B39" s="0"/>
       <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
+      <c r="D39" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
@@ -2203,7 +2278,7 @@
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
+      <c r="H40" s="0"/>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
@@ -2223,24 +2298,18 @@
       <c r="Y40" s="2"/>
       <c r="Z40" s="2"/>
     </row>
-    <row r="41" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="52.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0"/>
       <c r="B41" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C41" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E41" s="2" t="n">
-        <v>32</v>
-      </c>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
@@ -2261,17 +2330,17 @@
       <c r="Y41" s="2"/>
       <c r="Z41" s="2"/>
     </row>
-    <row r="42" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0"/>
       <c r="B42" s="3"/>
       <c r="C42" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>93</v>
       </c>
       <c r="E42" s="2" t="n">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
@@ -2297,17 +2366,17 @@
       <c r="Y42" s="2"/>
       <c r="Z42" s="2"/>
     </row>
-    <row r="43" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0"/>
       <c r="B43" s="3"/>
       <c r="C43" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>95</v>
       </c>
       <c r="E43" s="2" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
@@ -2333,17 +2402,17 @@
       <c r="Y43" s="2"/>
       <c r="Z43" s="2"/>
     </row>
-    <row r="44" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0"/>
       <c r="B44" s="3"/>
       <c r="C44" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>97</v>
       </c>
       <c r="E44" s="2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
@@ -2369,22 +2438,22 @@
       <c r="Y44" s="2"/>
       <c r="Z44" s="2"/>
     </row>
-    <row r="45" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0"/>
       <c r="B45" s="3"/>
       <c r="C45" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E45" s="2" t="s">
-        <v>100</v>
+      <c r="E45" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
@@ -2405,17 +2474,17 @@
       <c r="Y45" s="2"/>
       <c r="Z45" s="2"/>
     </row>
-    <row r="46" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0"/>
       <c r="B46" s="0"/>
       <c r="C46" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D46" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="E46" s="2" t="n">
-        <v>4</v>
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
@@ -2441,16 +2510,22 @@
       <c r="Y46" s="2"/>
       <c r="Z46" s="2"/>
     </row>
-    <row r="47" customFormat="false" ht="52.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0"/>
       <c r="B47" s="0"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
+      <c r="C47" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E47" s="2" t="n">
+        <v>4</v>
+      </c>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
@@ -2471,23 +2546,19 @@
       <c r="Y47" s="2"/>
       <c r="Z47" s="2"/>
     </row>
-    <row r="48" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="116.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0"/>
       <c r="B48" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D48" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E48" s="2" t="s">
-        <v>57</v>
-      </c>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
+      <c r="H48" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
@@ -2507,23 +2578,19 @@
       <c r="Y48" s="2"/>
       <c r="Z48" s="2"/>
     </row>
-    <row r="49" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0"/>
       <c r="C49" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E49" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="F49" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="E49" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
@@ -2544,19 +2611,23 @@
       <c r="Y49" s="2"/>
       <c r="Z49" s="2"/>
     </row>
-    <row r="50" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0"/>
       <c r="C50" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D50" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E50" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E50" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
+      <c r="F50" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
@@ -2577,16 +2648,20 @@
       <c r="Y50" s="2"/>
       <c r="Z50" s="2"/>
     </row>
-    <row r="51" customFormat="false" ht="116.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
+      <c r="C51" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>110</v>
+      </c>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
-      <c r="H51" s="2" t="s">
-        <v>111</v>
-      </c>
+      <c r="H51" s="0"/>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
@@ -2606,23 +2681,19 @@
       <c r="Y51" s="2"/>
       <c r="Z51" s="2"/>
     </row>
-    <row r="52" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="307.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0"/>
       <c r="B52" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D52" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E52" s="2" t="s">
-        <v>114</v>
-      </c>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
+      <c r="H52" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
@@ -2642,17 +2713,21 @@
       <c r="Y52" s="2"/>
       <c r="Z52" s="2"/>
     </row>
-    <row r="53" customFormat="false" ht="294.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0"/>
       <c r="B53" s="0"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
+      <c r="C53" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>116</v>
+      </c>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
-      <c r="H53" s="2" t="s">
-        <v>115</v>
-      </c>
+      <c r="H53" s="0"/>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
@@ -2675,7 +2750,7 @@
     <row r="54" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2"/>
       <c r="B54" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -2730,32 +2805,22 @@
       <c r="Y55" s="2"/>
       <c r="Z55" s="2"/>
     </row>
-    <row r="56" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="103.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D56" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E56" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H56" s="2"/>
-      <c r="I56" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="I56" s="2"/>
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
@@ -2778,27 +2843,25 @@
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>44</v>
+        <v>121</v>
+      </c>
+      <c r="E57" s="2" t="n">
+        <v>8</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H57" s="2"/>
       <c r="I57" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J57" s="2" t="s">
-        <v>22</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="J57" s="2"/>
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
       <c r="M57" s="2"/>
@@ -2816,27 +2879,31 @@
       <c r="Y57" s="2"/>
       <c r="Z57" s="2"/>
     </row>
-    <row r="58" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>122</v>
+        <v>46</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H58" s="2"/>
-      <c r="I58" s="2"/>
-      <c r="J58" s="2"/>
+      <c r="I58" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J58" s="2" t="s">
+        <v>123</v>
+      </c>
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
@@ -2858,19 +2925,19 @@
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
@@ -2892,17 +2959,25 @@
       <c r="Y59" s="2"/>
       <c r="Z59" s="2"/>
     </row>
-    <row r="60" customFormat="false" ht="103.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
-      <c r="G60" s="2"/>
-      <c r="H60" s="2" t="s">
-        <v>125</v>
-      </c>
+      <c r="C60" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H60" s="0"/>
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
@@ -2922,28 +2997,18 @@
       <c r="Y60" s="2"/>
       <c r="Z60" s="2"/>
     </row>
-    <row r="61" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E61" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="F61" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="G61" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
@@ -2968,25 +3033,23 @@
       <c r="A62" s="0"/>
       <c r="B62" s="0"/>
       <c r="C62" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="E62" s="2" t="s">
-        <v>44</v>
+      <c r="E62" s="2" t="n">
+        <v>5</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
-      <c r="J62" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="J62" s="2"/>
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
       <c r="M62" s="2"/>
@@ -3004,23 +3067,29 @@
       <c r="Y62" s="2"/>
       <c r="Z62" s="2"/>
     </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0"/>
       <c r="B63" s="0"/>
       <c r="C63" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D63" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F63" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E63" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="F63" s="2"/>
-      <c r="G63" s="2"/>
+      <c r="G63" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
-      <c r="J63" s="2"/>
+      <c r="J63" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
@@ -3038,24 +3107,20 @@
       <c r="Y63" s="2"/>
       <c r="Z63" s="2"/>
     </row>
-    <row r="64" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0"/>
       <c r="B64" s="0"/>
       <c r="C64" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G64" s="2" t="s">
-        <v>21</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
@@ -3076,11 +3141,11 @@
       <c r="Y64" s="2"/>
       <c r="Z64" s="2"/>
     </row>
-    <row r="65" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0"/>
       <c r="B65" s="0"/>
       <c r="C65" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D65" s="0" t="s">
         <v>134</v>
@@ -3089,10 +3154,10 @@
         <v>135</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
@@ -3118,7 +3183,7 @@
       <c r="A66" s="0"/>
       <c r="B66" s="0"/>
       <c r="C66" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D66" s="0" t="s">
         <v>136</v>
@@ -3127,11 +3192,12 @@
         <v>137</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>21</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="J66" s="2"/>
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
@@ -3153,45 +3219,45 @@
       <c r="A67" s="0"/>
       <c r="B67" s="0"/>
       <c r="C67" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D67" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="E67" s="5" t="s">
+      <c r="E67" s="0" t="s">
         <v>139</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0"/>
       <c r="B68" s="0"/>
       <c r="C68" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D68" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="E68" s="0" t="s">
+      <c r="E68" s="5" t="s">
         <v>141</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0"/>
       <c r="B69" s="0"/>
       <c r="C69" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D69" s="0" t="s">
         <v>142</v>
@@ -3200,17 +3266,17 @@
         <v>143</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0"/>
       <c r="B70" s="0"/>
       <c r="C70" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D70" s="0" t="s">
         <v>144</v>
@@ -3219,17 +3285,17 @@
         <v>145</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0"/>
       <c r="B71" s="0"/>
       <c r="C71" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D71" s="0" t="s">
         <v>146</v>
@@ -3238,278 +3304,274 @@
         <v>147</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0"/>
       <c r="B72" s="0"/>
       <c r="C72" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D72" s="0" t="s">
         <v>148</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0"/>
       <c r="B73" s="0"/>
       <c r="C73" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E73" s="0" t="s">
         <v>147</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0"/>
       <c r="B74" s="0"/>
       <c r="C74" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="F74" s="2"/>
-    </row>
-    <row r="75" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0"/>
-      <c r="B75" s="0"/>
-      <c r="C75" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D75" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="E75" s="0" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>149</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="2"/>
+      <c r="B75" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C75" s="0"/>
+      <c r="D75" s="0"/>
+      <c r="E75" s="0"/>
+      <c r="F75" s="2"/>
+    </row>
+    <row r="76" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0"/>
       <c r="B76" s="0"/>
-      <c r="C76" s="0"/>
-      <c r="D76" s="0"/>
-      <c r="E76" s="0"/>
-      <c r="F76" s="0"/>
-      <c r="G76" s="0"/>
+      <c r="C76" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>154</v>
+      </c>
       <c r="H76" s="0"/>
       <c r="I76" s="0"/>
-      <c r="J76" s="0"/>
-    </row>
-    <row r="77" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="2"/>
-      <c r="B77" s="2" t="s">
-        <v>152</v>
-      </c>
+    </row>
+    <row r="77" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C77" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0"/>
-      <c r="B78" s="0"/>
+        <v>156</v>
+      </c>
+      <c r="F77" s="0"/>
+      <c r="G77" s="0"/>
+      <c r="J77" s="0"/>
+    </row>
+    <row r="78" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C78" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C79" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D79" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E79" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D80" s="0"/>
-    </row>
-    <row r="81" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="2" t="s">
+      <c r="E78" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B79" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="D79" s="0"/>
+    </row>
+    <row r="80" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="2"/>
+      <c r="C80" s="2" t="s">
         <v>160</v>
       </c>
+      <c r="D80" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0"/>
       <c r="D81" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="2"/>
+        <v>163</v>
+      </c>
+      <c r="J81" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0"/>
+      <c r="B82" s="0"/>
       <c r="D82" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="E82" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B83" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C83" s="0"/>
+      <c r="D83" s="0"/>
+    </row>
+    <row r="84" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C84" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D84" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="E84" s="1" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="83" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0"/>
-      <c r="D83" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0"/>
-      <c r="B84" s="0"/>
-      <c r="C84" s="0"/>
-      <c r="D84" s="0"/>
-    </row>
-    <row r="85" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J84" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="2"/>
       <c r="B85" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="C85" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D85" s="0"/>
+    </row>
+    <row r="86" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0"/>
+      <c r="B86" s="2"/>
+      <c r="C86" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="D85" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D86" s="0"/>
-    </row>
-    <row r="87" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="2"/>
-      <c r="B87" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>160</v>
-      </c>
+      <c r="D86" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C87" s="2"/>
       <c r="D87" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="0"/>
-      <c r="B88" s="2"/>
-      <c r="C88" s="2"/>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D88" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D89" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="E89" s="6" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="91" customFormat="false" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B91" s="1" t="s">
         <v>174</v>
       </c>
+      <c r="E88" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B89" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C90" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C91" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C92" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C93" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="0"/>
-      <c r="B96" s="0"/>
-      <c r="C96" s="0"/>
-      <c r="D96" s="2"/>
-      <c r="E96" s="2"/>
-    </row>
-    <row r="97" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="B97" s="0"/>
-      <c r="C97" s="0"/>
-      <c r="D97" s="0"/>
-      <c r="E97" s="0"/>
-    </row>
+        <v>182</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0"/>
+      <c r="B94" s="0"/>
+    </row>
+    <row r="95" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B95" s="0"/>
+      <c r="C95" s="0"/>
+      <c r="D95" s="0"/>
+      <c r="E95" s="0"/>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4467,7 +4529,7 @@
     <row r="1052" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H47" r:id="rId1" display="https://arxiv.org/abs/1509.06264"/>
+    <hyperlink ref="H41" r:id="rId1" display="https://arxiv.org/abs/1509.06264"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4477,4 +4539,131 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1683673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.2908163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.8571428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.2551020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.4591836734694"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.3214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated many parameter descriptions
</commit_message>
<xml_diff>
--- a/SimCADO/simcado/docs/SimCADO_defaults.xlsx
+++ b/SimCADO/simcado/docs/SimCADO_defaults.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="250">
   <si>
     <t xml:space="preserve">Section</t>
   </si>
@@ -74,8 +74,9 @@
     <t xml:space="preserve">Point spread function</t>
   </si>
   <si>
-    <t xml:space="preserve">Currently waiting on SCAO PSFs for the default. If there are none ready, we will ship with the ESO LTAO PSFs from the 2012 AO study for a 42m mirror. 
-Other options include using the POPPY PSF simulator from the JWST to make PSFs on the fly</t>
+    <t xml:space="preserve">What happens before the deformable mirrors is a mystery to SimCADO. All SimCADO needs is the effective PSF for the chosen AO mode. 
+Currently SimCADO assumes a single PSF for the whole field. This will change when position dependent PSFs become available
+SCAO PSFs have been provided by Yann Clenet for the JHK. LTAO PSFs from ESOs 2012 study are included. Ideal (no atmosphere) generated by the JWST POPPY optics tool are also included.</t>
   </si>
   <si>
     <t xml:space="preserve">SCOPE</t>
@@ -84,35 +85,48 @@
     <t xml:space="preserve">SCOPE_PSF_FILE</t>
   </si>
   <si>
-    <t xml:space="preserve">data/PSF_LTAO.fits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESO E-ELT optics webpage (2012 study)</t>
+    <t xml:space="preserve">data/PSF_SCAO.fits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yann Clenet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.11.2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEEDED : MCAO PSF, SCAO position-dep PSFs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">im</t>
+  </si>
+  <si>
+    <t xml:space="preserve">["scao" (default), &lt;filename&gt;, "ltao", "mcao", "poppy"] import a PSF from a file.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atmospheric Dispersion Correction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of surfaces in the ADC is set to 8. A constant transmission curve of 0.98 is assumed for each of these surfaces, thus the total throughput of a perfectly functioning ADC is `0.98^8 = 0.85` over the wavelength range 0.5-3.0um
+SimCADO implements an inverse ADC. It assumes that the ADC corrects perfectly for the dispersion induced by the atmosphere. If the ADC isn't working as it should, i.e. `INST_ADC_PERFORMANCE` less than 100%, SimCADO calculates the distance an uncorrected image/slice would be from the centre of the FoV, then shifts the image/slice by `shift = AD * (1 - 0.01 * INST_ADC_PERFORMANCE)`. By calculating this shift for each slice in the spectral cube, SimCADO recreates the smearing effect of an imperfect ADC.
+What is needed is real model for how the ADC residuals affect the image on the focal plane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INST_ADC_PERFORMANCE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Best guess</t>
   </si>
   <si>
     <t xml:space="preserve">02.11.2016</t>
   </si>
   <si>
-    <t xml:space="preserve">im</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Atmospheric Dispersion Correction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of surfaces in the ADC is set to 8. A constant transmission curve of 0.98 is assumed for each of these surfaces, thus the total throughput of a perfectly functioning ADC is `0.98^8 = 0.85` over the wavelength range 0.5-3.0um
-SimCADO implements an inverse ADC. It assumes that the ADC corrects perfectly for the dispersion induced by the atmosphere. If the ADC isn't working as it should, i.e. `INST_ADC_PERFORMANCE` less than 100%, SimCADO calculates the distance an uncorrected image/slice would be from the centre of the FoV, then shifts the image/slice by `shift = AD * (1 - 0.01 * INST_ADC_PERFORMANCE)`. By calculating this shift for each slice in the spectral cube, SimCADO recreates the smearing effect of an imperfect ADC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INST_ADC_PERFORMANCE </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Best guess</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REAL DATA NEEDED</t>
+    <t xml:space="preserve">NEEDED : Model for ADC, unless % performance metric is OK. How does slip/give translate to FP shift?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[%] how well the ADC does its job</t>
   </si>
   <si>
     <t xml:space="preserve">INST_ADC_NUM_SURFACES </t>
@@ -121,7 +135,10 @@
     <t xml:space="preserve">Email from Ric</t>
   </si>
   <si>
-    <t xml:space="preserve">Source needed</t>
+    <t xml:space="preserve">NEEDED : Number of surfaces, unless a curve/number can be supplied for the whole ADC. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of surfaces in the ADC</t>
   </si>
   <si>
     <t xml:space="preserve">INST_ADC_TC </t>
@@ -130,7 +147,13 @@
     <t xml:space="preserve">data/TC_ADC.dat</t>
   </si>
   <si>
+    <t xml:space="preserve">NEEDED : Real TC or at least approx %. Is TC dependent on position of prisms?</t>
+  </si>
+  <si>
     <t xml:space="preserve">y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">transmission curve of the ADC</t>
   </si>
   <si>
     <t xml:space="preserve">Derotator</t>
@@ -144,10 +167,22 @@
     <t xml:space="preserve">INST_DEROT_PERFORMANCE</t>
   </si>
   <si>
+    <t xml:space="preserve">NEEDED : How do distances (mm, um) translate to FP angles (mas, arcsec)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[%] how well the derotator derotates</t>
+  </si>
+  <si>
     <t xml:space="preserve">INST_DEROT_PROFILE</t>
   </si>
   <si>
     <t xml:space="preserve">linear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEEDED : Is a linear shift OK? Whats the best model for this?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[linear, gaussian] the profile with which it does it's job</t>
   </si>
   <si>
     <t xml:space="preserve">MICADO transmission effects</t>
@@ -163,6 +198,12 @@
     <t xml:space="preserve">INST_NUM_MIRRORS</t>
   </si>
   <si>
+    <t xml:space="preserve">MICADO optical design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of reflecting surfaces in MICADO</t>
+  </si>
+  <si>
     <t xml:space="preserve">INST_MIRROR_TC</t>
   </si>
   <si>
@@ -170,6 +211,12 @@
   </si>
   <si>
     <t xml:space="preserve">ESO E-ELT technical database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEEDED : What coating materials are we going to use? Which possibilities?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If "default", INST_MIRROR_TC = SCOPE_M1_TC</t>
   </si>
   <si>
     <t xml:space="preserve">Filters</t>
@@ -195,9 +242,15 @@
     <t xml:space="preserve">data/TC_filter_Ks.dat</t>
   </si>
   <si>
+    <t xml:space="preserve">NEEDED : Which filters will be available</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cryostat window</t>
   </si>
   <si>
+    <t xml:space="preserve">The entrance window for MICADO. At the moment we assume a transmission of approx 95% per surface. </t>
+  </si>
+  <si>
     <t xml:space="preserve">INST_ENTR_NUM_SURFACES</t>
   </si>
   <si>
@@ -207,9 +260,15 @@
     <t xml:space="preserve">data/TC_window.dat</t>
   </si>
   <si>
+    <t xml:space="preserve">NEEDED : Ideally a transmission curve for the full window. Also acceptable is a single number. At the least, a meterial name/composition so that I can search</t>
+  </si>
+  <si>
     <t xml:space="preserve">Instrumental distorion</t>
   </si>
   <si>
+    <t xml:space="preserve">SimCADO shifts </t>
+  </si>
+  <si>
     <t xml:space="preserve">INST_DISTORTION_MAP</t>
   </si>
   <si>
@@ -234,6 +293,12 @@
     <t xml:space="preserve">data/TC_dichroic.dat</t>
   </si>
   <si>
+    <t xml:space="preserve">Currently we are assuming 100% transmission. What material?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[&lt;filename&gt;, "default"]</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pupil optics</t>
   </si>
   <si>
@@ -243,12 +308,21 @@
     <t xml:space="preserve">INST_PUPIL_NUM_SURFACES</t>
   </si>
   <si>
+    <t xml:space="preserve">Is the TC for a single or both surfaces?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of surfaces on the pupil window</t>
+  </si>
+  <si>
     <t xml:space="preserve">INST_PUPIL_TC</t>
   </si>
   <si>
     <t xml:space="preserve">data/TC_pupil.dat</t>
   </si>
   <si>
+    <t xml:space="preserve">NEEDED : Did I understand this will be Zerodur+Cr </t>
+  </si>
+  <si>
     <t xml:space="preserve">MICADO Detector effects</t>
   </si>
   <si>
@@ -262,6 +336,15 @@
   </si>
   <si>
     <t xml:space="preserve">data/TC_detector_H4RG.dat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can‘t remember where I got this from</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source needed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantum efficiency of detector.</t>
   </si>
   <si>
     <t xml:space="preserve">Chip noise characteristics</t>
@@ -278,15 +361,24 @@
     <t xml:space="preserve">yes</t>
   </si>
   <si>
+    <t xml:space="preserve">[yes/no]</t>
+  </si>
+  <si>
     <t xml:space="preserve">FPA_NOISE_PATH</t>
   </si>
   <si>
     <t xml:space="preserve">data/FPA_noise.fits</t>
   </si>
   <si>
+    <t xml:space="preserve">[default/generate/filename] if "generate": use NGHxRG to create a noise frame</t>
+  </si>
+  <si>
     <t xml:space="preserve">FPA_READOUT_MEDIAN</t>
   </si>
   <si>
+    <t xml:space="preserve">e-/px</t>
+  </si>
+  <si>
     <t xml:space="preserve">FPA_READOUT_STDEV</t>
   </si>
   <si>
@@ -296,6 +388,9 @@
     <t xml:space="preserve">0.01</t>
   </si>
   <si>
+    <t xml:space="preserve">e-/s/px</t>
+  </si>
+  <si>
     <t xml:space="preserve">FPA_DARK_STDEV</t>
   </si>
   <si>
@@ -305,44 +400,31 @@
     <t xml:space="preserve">FPA_GAIN</t>
   </si>
   <si>
+    <t xml:space="preserve">e- to ADU conversion</t>
+  </si>
+  <si>
     <t xml:space="preserve">FPA_WELL_DEPTH</t>
   </si>
   <si>
+    <t xml:space="preserve">number of photons collectable before pixel is full</t>
+  </si>
+  <si>
     <t xml:space="preserve">FPA_LINEARITY_CURVE</t>
   </si>
   <si>
+    <t xml:space="preserve">data/FPA_linearity.dat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[&lt;filename&gt;, "none", "default"]</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hawaii 4RG Simulator</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">These values are the defaults from the Hawaii xRG noise generator code (Rauscher 2015)
-[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://arxiv.org/abs/1509.06264</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">]()</t>
-    </r>
+    <t xml:space="preserve">These values are the defaults from the Hawaii xRG noise generator code (Rauscher 2015)</t>
   </si>
   <si>
     <t xml:space="preserve">HXRG</t>
@@ -398,16 +480,25 @@
     <t xml:space="preserve">FPA_PIXEL_MAP</t>
   </si>
   <si>
+    <t xml:space="preserve">path to a FITS file with the pixel sensitivity map</t>
+  </si>
+  <si>
     <t xml:space="preserve">FPA_DEAD_PIXELS</t>
   </si>
   <si>
-    <t xml:space="preserve">1%</t>
+    <t xml:space="preserve">1</t>
   </si>
   <si>
     <t xml:space="preserve">Simms+ 2007 for H2RG</t>
   </si>
   <si>
+    <t xml:space="preserve">[%] if FPA_PIXEL_MAP=none, a percentage of detector pixel which are dead</t>
+  </si>
+  <si>
     <t xml:space="preserve">FPA_DEAD_LINES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[%] if FPA_PIXEL_MAP=none, a percentage of detector lines which are dead</t>
   </si>
   <si>
     <t xml:space="preserve">Detector layout</t>
@@ -430,6 +521,9 @@
     <t xml:space="preserve">data/FPA_chip_layout_small.dat</t>
   </si>
   <si>
+    <t xml:space="preserve">["small", "centre", "wide", "zoom", "full", &lt;filename&gt;] description of the chip layout on the detector array</t>
+  </si>
+  <si>
     <t xml:space="preserve">MICADO Detector read modes</t>
   </si>
   <si>
@@ -440,28 +534,40 @@
   </si>
   <si>
     <t xml:space="preserve">The same mirror coating is assumed for the MAORY mirrors as for the E-ELT and MICADO
-Here we also assume 8x 1m class mirrors, held at ambient temperature emitting as grey bodies. The total surface area (`INST_MIRROR_AO_SUM_AREA`) of all mirrors in the AO system are used for the thermal background</t>
+Here we also assume 7x  mirrors, held at ambient temperature emitting as grey bodies. The total surface area (`INST_MIRROR_AO_SUM_AREA`) of all mirrors in the AO system are used for the thermal background</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INST_USE_AO_MIRROR_BG</t>
   </si>
   <si>
     <t xml:space="preserve">INST_NUM_AO_MIRRORS</t>
   </si>
   <si>
+    <t xml:space="preserve">REAL DATA NEEDED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of reflecting surfaces between telescope and instrument (i.e. MAORY)</t>
+  </si>
+  <si>
     <t xml:space="preserve">INST_MIRROR_AO_TC</t>
   </si>
   <si>
     <t xml:space="preserve">n</t>
   </si>
   <si>
-    <t xml:space="preserve">INST_MIRROR_AO_SUM_AREA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.28 m^2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INST_MIRROR_AO_TEMP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0 deg Celcius</t>
+    <t xml:space="preserve">If "default", INST_MIRROR_AO_TC = SCOPE_M1_TC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INST_AO_TEMPERATURE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deg Celsius - inside temp of AO module</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INST_MIRROR_AO_LIST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List of mirrors in the AO. </t>
   </si>
   <si>
     <t xml:space="preserve">Telescope optics</t>
@@ -470,70 +576,35 @@
     <t xml:space="preserve">E-ELT optical surfaces</t>
   </si>
   <si>
-    <t xml:space="preserve">SCOPE_NUM_MIRRORS</t>
+    <t xml:space="preserve">The optical surfaces for the telescope. SimCADO only cares about the transmission of the mirrors. MICADO only cares about the post-AO PSF, and so does SimCADO
+Telescope Jitter (wind, vibrations) and tracking drift are taken into account in a very basic fashion, similar to the ADC shift</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCOPE_M1_TC</t>
   </si>
   <si>
     <t xml:space="preserve">ESO E-ELT optics webpage</t>
   </si>
   <si>
-    <t xml:space="preserve">SCOPE_M1_TC</t>
+    <t xml:space="preserve">[&lt;filename&gt;, "default"] Mirror reflectance curve.</t>
   </si>
   <si>
     <t xml:space="preserve">SCOPE_M1_TEMP</t>
   </si>
   <si>
-    <t xml:space="preserve">SCOPE_M1_DIAMETER_OUT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCOPE_M1_DIAMETER_IN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCOPE_M2_DIAMETER_OUT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCOPE_M2_DIAMETER_IN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.545</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCOPE_M3_DIAMETER_OUT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCOPE_M3_DIAMETER_IN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCOPE_M4_DIAMETER_OUT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCOPE_M4_DIAMETER_IN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCOPE_M5_DIAMETER_OUT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCOPE_M5_DIAMETER_IN</t>
+    <t xml:space="preserve">Assumption that the outside temperature is around 0 deg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deg Celsius - temperature of mirror</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCOPE_MIRROR_LIST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data/EC_mirrors_scope.tbl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[&lt;filename&gt;, "default"] List of mirror sizes</t>
   </si>
   <si>
     <t xml:space="preserve">Wind jitter and telescope vibrations</t>
@@ -542,18 +613,24 @@
     <t xml:space="preserve">SCOPE_JITTER_FWHM</t>
   </si>
   <si>
-    <t xml:space="preserve">0.001 arcsec</t>
+    <t xml:space="preserve">0.001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[arcsec] gaussian telescope jitter (wind, tracking)</t>
   </si>
   <si>
     <t xml:space="preserve">SCOPE_DRIFT_DISTANCE</t>
   </si>
   <si>
-    <t xml:space="preserve">0 arcsec/sec</t>
+    <t xml:space="preserve">[arcsec/sec] the drift in tracking by the telescope</t>
   </si>
   <si>
     <t xml:space="preserve">SCOPE_DRIFT_PROFILE</t>
   </si>
   <si>
+    <t xml:space="preserve">[linear, gaussian] the drift profile. If linear, simulates when tracking is off. If gaussian, simulates rms distance of tracking errors</t>
+  </si>
+  <si>
     <t xml:space="preserve">Atmospheric Effects</t>
   </si>
   <si>
@@ -566,21 +643,33 @@
     <t xml:space="preserve">ATMO_USE_ATMO_BG</t>
   </si>
   <si>
+    <t xml:space="preserve">[yes/no] </t>
+  </si>
+  <si>
     <t xml:space="preserve">ATMO_EC</t>
   </si>
   <si>
     <t xml:space="preserve">data/skytable.fits</t>
   </si>
   <si>
+    <t xml:space="preserve">SkyCalc Uni IBK</t>
+  </si>
+  <si>
     <t xml:space="preserve">ec</t>
   </si>
   <si>
+    <t xml:space="preserve">[&lt;filename&gt;, "default", "none"] for atmospheric emission curve.</t>
+  </si>
+  <si>
     <t xml:space="preserve">ATMO_BG_MAGNITUDE</t>
   </si>
   <si>
     <t xml:space="preserve">data/EC_sky_magnitude.dat</t>
   </si>
   <si>
+    <t xml:space="preserve">If ATMO_EC is "none": set ATMO_BG_MAGNITUDE for the simulation filter. </t>
+  </si>
+  <si>
     <t xml:space="preserve">Transmission</t>
   </si>
   <si>
@@ -590,43 +679,61 @@
     <t xml:space="preserve">tc</t>
   </si>
   <si>
+    <t xml:space="preserve">[&lt;filename&gt;, "default"] for atmospheric transmission curve</t>
+  </si>
+  <si>
     <t xml:space="preserve">Atmospheric conditions</t>
   </si>
   <si>
     <t xml:space="preserve">ATMO_TEMPERATURE</t>
   </si>
   <si>
+    <t xml:space="preserve">deg Celcius</t>
+  </si>
+  <si>
     <t xml:space="preserve">ATMO_PRESSURE</t>
   </si>
   <si>
-    <t xml:space="preserve">750 millibar</t>
+    <t xml:space="preserve">millibar</t>
   </si>
   <si>
     <t xml:space="preserve">ATMO_REL_HUMIDITY</t>
   </si>
   <si>
-    <t xml:space="preserve">60%</t>
+    <t xml:space="preserve">60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%</t>
   </si>
   <si>
     <t xml:space="preserve">Telescope location parameters</t>
   </si>
   <si>
+    <t xml:space="preserve">Currently only used for getting the atmospheric dispersion</t>
+  </si>
+  <si>
     <t xml:space="preserve">SCOPE_ALTITUDE</t>
   </si>
   <si>
-    <t xml:space="preserve">3060 m</t>
+    <t xml:space="preserve">wikipedia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meters above sea level</t>
   </si>
   <si>
     <t xml:space="preserve">SCOPE_LATITUDE</t>
   </si>
   <si>
-    <t xml:space="preserve">-24.589167 deg</t>
+    <t xml:space="preserve">-24.589167</t>
+  </si>
+  <si>
+    <t xml:space="preserve">decimal degrees</t>
   </si>
   <si>
     <t xml:space="preserve">SCOPE_LONGITUDE</t>
   </si>
   <si>
-    <t xml:space="preserve">-70.192222 deg</t>
+    <t xml:space="preserve">-70.192222</t>
   </si>
   <si>
     <t xml:space="preserve">EOF</t>
@@ -702,12 +809,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
     <numFmt numFmtId="166" formatCode="@"/>
+    <numFmt numFmtId="167" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -732,13 +840,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Cambria"/>
       <family val="1"/>
       <charset val="1"/>
@@ -786,7 +887,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -811,8 +912,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -832,31 +945,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z126"/>
+  <dimension ref="A1:Z86"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E89" activeCellId="0" sqref="E89"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B17" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="33.4795918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="32.3979591836735"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="47.9234693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="26.3214285714286"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="20.5918367346939"/>
-    <col collapsed="false" hidden="false" max="14" min="12" style="1" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="23.8316326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="1" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.25"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="31.7244897959184"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="45.6275510204082"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="14" min="12" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="1" width="13.0918367346939"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -914,7 +1027,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="77.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="159.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -931,7 +1044,7 @@
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="0"/>
-      <c r="K2" s="2"/>
+      <c r="K2" s="0"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -948,7 +1061,7 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="67.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
@@ -967,11 +1080,15 @@
         <v>22</v>
       </c>
       <c r="H3" s="0"/>
-      <c r="I3" s="2"/>
+      <c r="I3" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="J3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -988,10 +1105,10 @@
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
     </row>
-    <row r="4" customFormat="false" ht="205.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="290.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -999,7 +1116,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="I4" s="0"/>
       <c r="J4" s="2"/>
@@ -1020,30 +1137,32 @@
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
     </row>
-    <row r="5" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="67.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E5" s="2" t="n">
         <v>100</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="K5" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -1060,30 +1179,32 @@
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="67.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2"/>
       <c r="B6" s="0"/>
       <c r="C6" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E6" s="2" t="n">
         <v>8</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
+      <c r="K6" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -1100,32 +1221,34 @@
       <c r="Y6" s="2"/>
       <c r="Z6" s="2"/>
     </row>
-    <row r="7" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="54.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="H7" s="0"/>
       <c r="I7" s="2" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K7" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -1142,10 +1265,10 @@
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
     </row>
-    <row r="8" customFormat="false" ht="141.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="159.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -1153,7 +1276,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -1174,30 +1297,32 @@
       <c r="Y8" s="2"/>
       <c r="Z8" s="2"/>
     </row>
-    <row r="9" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="54.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="E9" s="2" t="n">
         <v>100</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
+      <c r="K9" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -1214,30 +1339,32 @@
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
     </row>
-    <row r="10" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="41.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="H10" s="0"/>
       <c r="I10" s="2" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
+      <c r="K10" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
@@ -1254,12 +1381,12 @@
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
     </row>
-    <row r="11" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="106.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -1267,7 +1394,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -1288,30 +1415,30 @@
       <c r="Y11" s="2"/>
       <c r="Z11" s="2"/>
     </row>
-    <row r="12" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="41.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="E12" s="2" t="n">
         <v>11</v>
       </c>
       <c r="F12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="H12" s="2"/>
-      <c r="I12" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="I12" s="2"/>
       <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
+      <c r="K12" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
@@ -1328,32 +1455,34 @@
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
     </row>
-    <row r="13" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="41.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="H13" s="0"/>
       <c r="I13" s="2" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K13" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -1370,10 +1499,10 @@
       <c r="Y13" s="2"/>
       <c r="Z13" s="2"/>
     </row>
-    <row r="14" customFormat="false" ht="230.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="251.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -1381,7 +1510,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1402,28 +1531,30 @@
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
     </row>
-    <row r="15" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="H15" s="0"/>
-      <c r="I15" s="2"/>
+      <c r="I15" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="J15" s="2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
@@ -1442,17 +1573,19 @@
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
     </row>
-    <row r="16" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="41.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="H16" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -1472,23 +1605,23 @@
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
     </row>
-    <row r="17" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="E17" s="2" t="n">
         <v>4</v>
       </c>
       <c r="F17" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -1510,28 +1643,30 @@
       <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
     </row>
-    <row r="18" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="106.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
+      <c r="I18" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="J18" s="2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
@@ -1550,17 +1685,19 @@
       <c r="Y18" s="2"/>
       <c r="Z18" s="2"/>
     </row>
-    <row r="19" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
+      <c r="H19" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
@@ -1580,23 +1717,23 @@
       <c r="Y19" s="2"/>
       <c r="Z19" s="2"/>
     </row>
-    <row r="20" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="H20" s="0"/>
       <c r="I20" s="2"/>
@@ -1618,10 +1755,10 @@
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
     </row>
-    <row r="21" customFormat="false" ht="37.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="41.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -1629,7 +1766,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="1" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -1650,23 +1787,23 @@
       <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>
     </row>
-    <row r="22" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="E22" s="2" t="n">
         <v>2</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="H22" s="0"/>
       <c r="I22" s="2"/>
@@ -1688,28 +1825,32 @@
       <c r="Y22" s="2"/>
       <c r="Z22" s="2"/>
     </row>
-    <row r="23" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="54.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="H23" s="0"/>
-      <c r="I23" s="2"/>
+      <c r="I23" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="J23" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K23" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -1726,10 +1867,10 @@
       <c r="Y23" s="2"/>
       <c r="Z23" s="2"/>
     </row>
-    <row r="24" customFormat="false" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -1737,7 +1878,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="1" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -1758,30 +1899,32 @@
       <c r="Y24" s="2"/>
       <c r="Z24" s="2"/>
     </row>
-    <row r="25" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="E25" s="2" t="n">
         <v>2</v>
       </c>
       <c r="F25" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G25" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="H25" s="0"/>
       <c r="I25" s="2" t="s">
-        <v>32</v>
+        <v>89</v>
       </c>
       <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
+      <c r="K25" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -1798,30 +1941,32 @@
       <c r="Y25" s="2"/>
       <c r="Z25" s="2"/>
     </row>
-    <row r="26" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="41.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="H26" s="0"/>
       <c r="I26" s="2" t="s">
-        <v>29</v>
+        <v>93</v>
       </c>
       <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
+      <c r="K26" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -1838,12 +1983,12 @@
       <c r="Y26" s="2"/>
       <c r="Z26" s="2"/>
     </row>
-    <row r="27" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -1870,28 +2015,32 @@
       <c r="Y27" s="2"/>
       <c r="Z27" s="2"/>
     </row>
-    <row r="28" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2"/>
       <c r="B28" s="0"/>
       <c r="C28" s="2" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F28" s="2"/>
+        <v>98</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2" t="s">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K28" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
@@ -1908,10 +2057,10 @@
       <c r="Y28" s="2"/>
       <c r="Z28" s="2"/>
     </row>
-    <row r="29" customFormat="false" ht="141.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="159.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2"/>
       <c r="B29" s="1" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="3"/>
@@ -1919,7 +2068,7 @@
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2" t="s">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
@@ -1940,24 +2089,26 @@
       <c r="Y29" s="2"/>
       <c r="Z29" s="2"/>
     </row>
-    <row r="30" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2"/>
       <c r="B30" s="0"/>
       <c r="C30" s="2" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>77</v>
+        <v>104</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>78</v>
+        <v>105</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
+      <c r="K30" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
@@ -1974,24 +2125,28 @@
       <c r="Y30" s="2"/>
       <c r="Z30" s="2"/>
     </row>
-    <row r="31" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="67.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2"/>
       <c r="B31" s="0"/>
       <c r="C31" s="2" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>79</v>
+        <v>107</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>80</v>
+        <v>108</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
+      <c r="J31" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>109</v>
+      </c>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -2008,14 +2163,14 @@
       <c r="Y31" s="2"/>
       <c r="Z31" s="2"/>
     </row>
-    <row r="32" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2"/>
       <c r="B32" s="0"/>
       <c r="C32" s="2" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>81</v>
+        <v>110</v>
       </c>
       <c r="E32" s="2" t="n">
         <v>4</v>
@@ -2025,7 +2180,9 @@
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
+      <c r="K32" s="2" t="s">
+        <v>111</v>
+      </c>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -2042,14 +2199,14 @@
       <c r="Y32" s="2"/>
       <c r="Z32" s="2"/>
     </row>
-    <row r="33" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2"/>
       <c r="B33" s="0"/>
       <c r="C33" s="2" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>82</v>
+        <v>112</v>
       </c>
       <c r="E33" s="2" t="n">
         <v>1</v>
@@ -2059,7 +2216,9 @@
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
+      <c r="K33" s="2" t="s">
+        <v>111</v>
+      </c>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -2076,24 +2235,26 @@
       <c r="Y33" s="2"/>
       <c r="Z33" s="2"/>
     </row>
-    <row r="34" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2"/>
       <c r="B34" s="0"/>
       <c r="C34" s="2" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>84</v>
+        <v>114</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
+      <c r="K34" s="2" t="s">
+        <v>115</v>
+      </c>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -2110,24 +2271,26 @@
       <c r="Y34" s="2"/>
       <c r="Z34" s="2"/>
     </row>
-    <row r="35" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2"/>
       <c r="B35" s="0"/>
       <c r="C35" s="2" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>84</v>
+        <v>114</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="0"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
+      <c r="K35" s="2" t="s">
+        <v>115</v>
+      </c>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -2147,7 +2310,7 @@
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2"/>
       <c r="B36" s="0" t="s">
-        <v>86</v>
+        <v>117</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -2174,12 +2337,12 @@
       <c r="Y36" s="2"/>
       <c r="Z36" s="2"/>
     </row>
-    <row r="37" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2"/>
       <c r="B37" s="0"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
-        <v>87</v>
+        <v>118</v>
       </c>
       <c r="E37" s="2" t="n">
         <v>1</v>
@@ -2189,7 +2352,9 @@
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
+      <c r="K37" s="2" t="s">
+        <v>119</v>
+      </c>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -2206,12 +2371,12 @@
       <c r="Y37" s="2"/>
       <c r="Z37" s="2"/>
     </row>
-    <row r="38" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="41.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2"/>
       <c r="B38" s="0"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
-        <v>88</v>
+        <v>120</v>
       </c>
       <c r="E38" s="4" t="n">
         <v>100000</v>
@@ -2221,7 +2386,9 @@
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
+      <c r="K38" s="2" t="s">
+        <v>121</v>
+      </c>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -2238,22 +2405,26 @@
       <c r="Y38" s="2"/>
       <c r="Z38" s="2"/>
     </row>
-    <row r="39" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2"/>
       <c r="B39" s="0"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
-        <v>89</v>
+        <v>122</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>58</v>
+        <v>123</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
+      <c r="J39" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>125</v>
+      </c>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -2279,7 +2450,7 @@
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="0"/>
-      <c r="I40" s="2"/>
+      <c r="I40" s="0"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
@@ -2298,10 +2469,10 @@
       <c r="Y40" s="2"/>
       <c r="Z40" s="2"/>
     </row>
-    <row r="41" customFormat="false" ht="52.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0"/>
       <c r="B41" s="3" t="s">
-        <v>90</v>
+        <v>126</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -2309,7 +2480,7 @@
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2" t="s">
-        <v>91</v>
+        <v>127</v>
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
@@ -2330,14 +2501,14 @@
       <c r="Y41" s="2"/>
       <c r="Z41" s="2"/>
     </row>
-    <row r="42" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0"/>
       <c r="B42" s="3"/>
       <c r="C42" s="2" t="s">
-        <v>92</v>
+        <v>128</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="E42" s="2" t="n">
         <v>32</v>
@@ -2345,7 +2516,7 @@
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2" t="s">
-        <v>94</v>
+        <v>130</v>
       </c>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
@@ -2366,14 +2537,14 @@
       <c r="Y42" s="2"/>
       <c r="Z42" s="2"/>
     </row>
-    <row r="43" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0"/>
       <c r="B43" s="3"/>
       <c r="C43" s="2" t="s">
-        <v>92</v>
+        <v>128</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="E43" s="2" t="n">
         <v>8</v>
@@ -2381,7 +2552,7 @@
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2" t="s">
-        <v>96</v>
+        <v>132</v>
       </c>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
@@ -2402,14 +2573,14 @@
       <c r="Y43" s="2"/>
       <c r="Z43" s="2"/>
     </row>
-    <row r="44" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0"/>
       <c r="B44" s="3"/>
       <c r="C44" s="2" t="s">
-        <v>92</v>
+        <v>128</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>97</v>
+        <v>133</v>
       </c>
       <c r="E44" s="2" t="n">
         <v>3</v>
@@ -2417,7 +2588,7 @@
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2" t="s">
-        <v>98</v>
+        <v>134</v>
       </c>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
@@ -2438,14 +2609,14 @@
       <c r="Y44" s="2"/>
       <c r="Z44" s="2"/>
     </row>
-    <row r="45" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0"/>
       <c r="B45" s="3"/>
       <c r="C45" s="2" t="s">
-        <v>92</v>
+        <v>128</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>99</v>
+        <v>135</v>
       </c>
       <c r="E45" s="2" t="n">
         <v>1</v>
@@ -2453,7 +2624,7 @@
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2" t="s">
-        <v>100</v>
+        <v>136</v>
       </c>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
@@ -2474,22 +2645,22 @@
       <c r="Y45" s="2"/>
       <c r="Z45" s="2"/>
     </row>
-    <row r="46" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0"/>
       <c r="B46" s="0"/>
       <c r="C46" s="2" t="s">
-        <v>92</v>
+        <v>128</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>101</v>
+        <v>137</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>102</v>
+        <v>138</v>
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2" t="s">
-        <v>103</v>
+        <v>139</v>
       </c>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
@@ -2510,14 +2681,14 @@
       <c r="Y46" s="2"/>
       <c r="Z46" s="2"/>
     </row>
-    <row r="47" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0"/>
       <c r="B47" s="0"/>
       <c r="C47" s="2" t="s">
-        <v>92</v>
+        <v>128</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>104</v>
+        <v>140</v>
       </c>
       <c r="E47" s="2" t="n">
         <v>4</v>
@@ -2525,7 +2696,7 @@
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2" t="s">
-        <v>105</v>
+        <v>141</v>
       </c>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
@@ -2546,10 +2717,10 @@
       <c r="Y47" s="2"/>
       <c r="Z47" s="2"/>
     </row>
-    <row r="48" customFormat="false" ht="116.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="133.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0"/>
       <c r="B48" s="1" t="s">
-        <v>106</v>
+        <v>142</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -2557,7 +2728,7 @@
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
@@ -2578,23 +2749,26 @@
       <c r="Y48" s="2"/>
       <c r="Z48" s="2"/>
     </row>
-    <row r="49" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="41.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0"/>
+      <c r="B49" s="0"/>
       <c r="C49" s="2" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>108</v>
+        <v>144</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
-      <c r="K49" s="2"/>
+      <c r="K49" s="2" t="s">
+        <v>145</v>
+      </c>
       <c r="L49" s="2"/>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -2611,27 +2785,30 @@
       <c r="Y49" s="2"/>
       <c r="Z49" s="2"/>
     </row>
-    <row r="50" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="67.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0"/>
+      <c r="B50" s="0"/>
       <c r="C50" s="2" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>109</v>
+        <v>146</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>110</v>
+        <v>147</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>111</v>
+        <v>148</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
-      <c r="K50" s="2"/>
+      <c r="K50" s="6" t="s">
+        <v>149</v>
+      </c>
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -2648,23 +2825,26 @@
       <c r="Y50" s="2"/>
       <c r="Z50" s="2"/>
     </row>
-    <row r="51" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="67.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0"/>
+      <c r="B51" s="0"/>
       <c r="C51" s="2" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>112</v>
+        <v>150</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>110</v>
+        <v>147</v>
       </c>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
       <c r="H51" s="0"/>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
-      <c r="K51" s="2"/>
+      <c r="K51" s="2" t="s">
+        <v>151</v>
+      </c>
       <c r="L51" s="2"/>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
@@ -2681,10 +2861,10 @@
       <c r="Y51" s="2"/>
       <c r="Z51" s="2"/>
     </row>
-    <row r="52" customFormat="false" ht="307.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="316.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0"/>
       <c r="B52" s="1" t="s">
-        <v>113</v>
+        <v>152</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -2692,7 +2872,7 @@
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2" t="s">
-        <v>114</v>
+        <v>153</v>
       </c>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
@@ -2713,24 +2893,26 @@
       <c r="Y52" s="2"/>
       <c r="Z52" s="2"/>
     </row>
-    <row r="53" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="80.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0"/>
       <c r="B53" s="0"/>
       <c r="C53" s="2" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>115</v>
+        <v>154</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>116</v>
+        <v>155</v>
       </c>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
       <c r="H53" s="0"/>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
-      <c r="K53" s="2"/>
+      <c r="K53" s="2" t="s">
+        <v>156</v>
+      </c>
       <c r="L53" s="2"/>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
@@ -2747,10 +2929,10 @@
       <c r="Y53" s="2"/>
       <c r="Z53" s="2"/>
     </row>
-    <row r="54" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2"/>
       <c r="B54" s="2" t="s">
-        <v>117</v>
+        <v>157</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -2805,12 +2987,12 @@
       <c r="Y55" s="2"/>
       <c r="Z55" s="2"/>
     </row>
-    <row r="56" customFormat="false" ht="103.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="119.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>118</v>
+        <v>158</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>119</v>
+        <v>159</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -2818,7 +3000,7 @@
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2" t="s">
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
@@ -2839,30 +3021,24 @@
       <c r="Y56" s="2"/>
       <c r="Z56" s="2"/>
     </row>
-    <row r="57" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E57" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G57" s="2" t="s">
-        <v>22</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
       <c r="H57" s="2"/>
-      <c r="I57" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="I57" s="2"/>
       <c r="J57" s="2"/>
-      <c r="K57" s="2"/>
+      <c r="K57" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="L57" s="2"/>
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
@@ -2879,32 +3055,32 @@
       <c r="Y57" s="2"/>
       <c r="Z57" s="2"/>
     </row>
-    <row r="58" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="67.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>46</v>
+        <v>162</v>
+      </c>
+      <c r="E58" s="2" t="n">
+        <v>7</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="H58" s="2"/>
       <c r="I58" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J58" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="K58" s="2"/>
+        <v>163</v>
+      </c>
+      <c r="J58" s="2"/>
+      <c r="K58" s="2" t="s">
+        <v>164</v>
+      </c>
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
@@ -2921,28 +3097,34 @@
       <c r="Y58" s="2"/>
       <c r="Z58" s="2"/>
     </row>
-    <row r="59" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="41.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>124</v>
+        <v>165</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>125</v>
+        <v>59</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="H59" s="2"/>
-      <c r="I59" s="2"/>
-      <c r="J59" s="2"/>
-      <c r="K59" s="2"/>
+      <c r="I59" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="J59" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="K59" s="2" t="s">
+        <v>167</v>
+      </c>
       <c r="L59" s="2"/>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
@@ -2959,28 +3141,30 @@
       <c r="Y59" s="2"/>
       <c r="Z59" s="2"/>
     </row>
-    <row r="60" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>127</v>
+        <v>168</v>
+      </c>
+      <c r="E60" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="H60" s="0"/>
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
-      <c r="K60" s="2"/>
+      <c r="K60" s="2" t="s">
+        <v>169</v>
+      </c>
       <c r="L60" s="2"/>
       <c r="M60" s="2"/>
       <c r="N60" s="2"/>
@@ -2997,22 +3181,24 @@
       <c r="Y60" s="2"/>
       <c r="Z60" s="2"/>
     </row>
-    <row r="61" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
+    <row r="61" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="2"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>170</v>
+      </c>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
-      <c r="H61" s="2"/>
+      <c r="H61" s="0"/>
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
-      <c r="K61" s="2"/>
+      <c r="K61" s="2" t="s">
+        <v>171</v>
+      </c>
       <c r="L61" s="2"/>
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
@@ -3029,25 +3215,21 @@
       <c r="Y61" s="2"/>
       <c r="Z61" s="2"/>
     </row>
-    <row r="62" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0"/>
-      <c r="B62" s="0"/>
-      <c r="C62" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E62" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G62" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H62" s="2"/>
+    <row r="62" customFormat="false" ht="106.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2" t="s">
+        <v>174</v>
+      </c>
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
@@ -3067,30 +3249,32 @@
       <c r="Y62" s="2"/>
       <c r="Z62" s="2"/>
     </row>
-    <row r="63" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="41.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0"/>
       <c r="B63" s="0"/>
       <c r="C63" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>132</v>
+        <v>175</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>131</v>
+        <v>176</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
       <c r="J63" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K63" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="K63" s="2" t="s">
+        <v>177</v>
+      </c>
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
@@ -3107,24 +3291,28 @@
       <c r="Y63" s="2"/>
       <c r="Z63" s="2"/>
     </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="41.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0"/>
       <c r="B64" s="0"/>
       <c r="C64" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="E64" s="0" t="s">
-        <v>127</v>
+        <v>178</v>
+      </c>
+      <c r="E64" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
-      <c r="I64" s="2"/>
+      <c r="I64" s="2" t="s">
+        <v>179</v>
+      </c>
       <c r="J64" s="2"/>
-      <c r="K64" s="2"/>
+      <c r="K64" s="2" t="s">
+        <v>180</v>
+      </c>
       <c r="L64" s="2"/>
       <c r="M64" s="2"/>
       <c r="N64" s="2"/>
@@ -3141,28 +3329,30 @@
       <c r="Y64" s="2"/>
       <c r="Z64" s="2"/>
     </row>
-    <row r="65" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="41.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0"/>
       <c r="B65" s="0"/>
       <c r="C65" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>134</v>
+        <v>181</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>135</v>
+        <v>182</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>131</v>
+        <v>176</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
-      <c r="K65" s="2"/>
+      <c r="K65" s="2" t="s">
+        <v>183</v>
+      </c>
       <c r="L65" s="2"/>
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
@@ -3179,1358 +3369,334 @@
       <c r="Y65" s="2"/>
       <c r="Z65" s="2"/>
     </row>
-    <row r="66" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0"/>
-      <c r="B66" s="0"/>
-      <c r="C66" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D66" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="E66" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G66" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J66" s="2"/>
-      <c r="K66" s="2"/>
-      <c r="L66" s="2"/>
-      <c r="M66" s="2"/>
-      <c r="N66" s="2"/>
-      <c r="O66" s="2"/>
-      <c r="P66" s="2"/>
-      <c r="Q66" s="2"/>
-      <c r="R66" s="2"/>
-      <c r="S66" s="2"/>
-      <c r="T66" s="2"/>
-      <c r="U66" s="2"/>
-      <c r="V66" s="2"/>
-      <c r="W66" s="2"/>
-      <c r="X66" s="2"/>
-      <c r="Y66" s="2"/>
-      <c r="Z66" s="2"/>
-    </row>
-    <row r="67" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="41.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="2"/>
+      <c r="B66" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C66" s="0"/>
+      <c r="D66" s="0"/>
+      <c r="E66" s="0"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="0"/>
+      <c r="H66" s="0"/>
+      <c r="I66" s="0"/>
+      <c r="J66" s="0"/>
+    </row>
+    <row r="67" customFormat="false" ht="41.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0"/>
       <c r="B67" s="0"/>
       <c r="C67" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D67" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="E67" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G67" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D67" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E67" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="F67" s="0"/>
+      <c r="G67" s="0"/>
+      <c r="H67" s="0"/>
+      <c r="I67" s="0"/>
+      <c r="J67" s="0"/>
+      <c r="K67" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="41.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0"/>
       <c r="B68" s="0"/>
       <c r="C68" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D68" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="E68" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G68" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D68" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F68" s="0"/>
+      <c r="G68" s="0"/>
+      <c r="J68" s="0"/>
+      <c r="K68" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="93.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0"/>
       <c r="B69" s="0"/>
       <c r="C69" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D69" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="E69" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="F69" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G69" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0"/>
-      <c r="B70" s="0"/>
-      <c r="C70" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D70" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="E70" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G70" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0"/>
+      <c r="D69" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J69" s="0"/>
+      <c r="K69" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C70" s="0"/>
+      <c r="D70" s="0"/>
+      <c r="E70" s="0"/>
+      <c r="J70" s="0"/>
+    </row>
+    <row r="71" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="2"/>
       <c r="B71" s="0"/>
-      <c r="C71" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D71" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="E71" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="F71" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G71" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C71" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="J71" s="0"/>
+      <c r="K71" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="54.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0"/>
       <c r="B72" s="0"/>
-      <c r="C72" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D72" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="E72" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G72" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C72" s="0"/>
+      <c r="D72" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="G72" s="8" t="n">
+        <v>42370</v>
+      </c>
+      <c r="J72" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="K72" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0"/>
       <c r="B73" s="0"/>
-      <c r="C73" s="1" t="s">
+      <c r="C73" s="0"/>
+      <c r="D73" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="J73" s="0"/>
+      <c r="K73" s="0" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0"/>
+      <c r="B74" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C74" s="0"/>
+      <c r="D74" s="0"/>
+      <c r="E74" s="0"/>
+      <c r="J74" s="0"/>
+    </row>
+    <row r="75" customFormat="false" ht="41.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0"/>
+      <c r="B75" s="0"/>
+      <c r="C75" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D75" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="G75" s="8" t="n">
+        <v>42370</v>
+      </c>
+      <c r="J75" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="K75" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="2"/>
+      <c r="B76" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C76" s="0"/>
+      <c r="D76" s="0"/>
+      <c r="E76" s="0"/>
+    </row>
+    <row r="77" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0"/>
+      <c r="B77" s="2"/>
+      <c r="C77" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E77" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K77" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0"/>
+      <c r="B78" s="0"/>
+      <c r="C78" s="2"/>
+      <c r="D78" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E78" s="1" t="n">
+        <v>750</v>
+      </c>
+      <c r="K78" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0"/>
+      <c r="B79" s="0"/>
+      <c r="C79" s="0"/>
+      <c r="D79" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E79" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="K79" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0"/>
+      <c r="B80" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C80" s="0"/>
+      <c r="D80" s="0"/>
+      <c r="E80" s="0"/>
+      <c r="H80" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0"/>
+      <c r="B81" s="0"/>
+      <c r="C81" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D73" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="E73" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G73" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0"/>
-      <c r="B74" s="0"/>
-      <c r="C74" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D74" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="E74" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G74" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="2"/>
-      <c r="B75" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C75" s="0"/>
-      <c r="D75" s="0"/>
-      <c r="E75" s="0"/>
-      <c r="F75" s="2"/>
-    </row>
-    <row r="76" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0"/>
-      <c r="B76" s="0"/>
-      <c r="C76" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="H76" s="0"/>
-      <c r="I76" s="0"/>
-    </row>
-    <row r="77" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C77" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="F77" s="0"/>
-      <c r="G77" s="0"/>
-      <c r="J77" s="0"/>
-    </row>
-    <row r="78" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C78" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="D79" s="0"/>
-    </row>
-    <row r="80" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="2"/>
-      <c r="C80" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0"/>
       <c r="D81" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="J81" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>219</v>
+      </c>
+      <c r="E81" s="1" t="n">
+        <v>3060</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G81" s="8" t="n">
+        <v>42690</v>
+      </c>
+      <c r="K81" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0"/>
       <c r="B82" s="0"/>
+      <c r="C82" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="D82" s="1" t="s">
-        <v>165</v>
+        <v>222</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C83" s="0"/>
-      <c r="D83" s="0"/>
-    </row>
-    <row r="84" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C84" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="D84" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="J84" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="2"/>
-      <c r="B85" s="2" t="s">
-        <v>170</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G82" s="8" t="n">
+        <v>42690</v>
+      </c>
+      <c r="K82" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0"/>
+      <c r="B83" s="0"/>
+      <c r="C83" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G83" s="8" t="n">
+        <v>42690</v>
+      </c>
+      <c r="K83" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0"/>
+      <c r="B84" s="0"/>
+      <c r="C84" s="0"/>
+      <c r="D84" s="0"/>
+      <c r="E84" s="0"/>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0"/>
+      <c r="B85" s="0"/>
+      <c r="C85" s="0"/>
       <c r="D85" s="0"/>
-    </row>
-    <row r="86" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0"/>
-      <c r="B86" s="2"/>
-      <c r="C86" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C87" s="2"/>
-      <c r="D87" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D88" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E88" s="6" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B89" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C90" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C91" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C92" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="0"/>
-      <c r="B94" s="0"/>
-    </row>
-    <row r="95" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="B95" s="0"/>
-      <c r="C95" s="0"/>
-      <c r="D95" s="0"/>
-      <c r="E95" s="0"/>
-    </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="300" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="305" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="306" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="307" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="308" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="309" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="310" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="311" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="312" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="315" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="316" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="317" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="318" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="319" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="320" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="321" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="322" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="323" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="324" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="325" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="326" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="327" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="328" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="329" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="330" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="331" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="332" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="333" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="334" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="335" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="336" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="337" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="339" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="340" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="341" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="342" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="343" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="344" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="345" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="346" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="347" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="348" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="349" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="350" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="351" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="352" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="353" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="354" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="355" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="356" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="357" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="358" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="359" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="360" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="361" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="362" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="363" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="364" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="365" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="366" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="367" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="368" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="369" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="370" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="371" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="372" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="373" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="374" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="375" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="376" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="377" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="378" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="379" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="380" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="381" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="382" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="383" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="384" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="385" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="386" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="387" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="388" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="389" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="390" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="391" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="392" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="393" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="394" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="395" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="396" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="397" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="398" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="399" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="400" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="401" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="402" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="403" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="404" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="405" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="406" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="407" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="408" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="409" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="410" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="411" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="412" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="413" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="414" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="415" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="416" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="417" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="418" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="419" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="420" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="421" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="422" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="423" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="424" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="425" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="426" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="427" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="428" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="429" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="430" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="431" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="432" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="433" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="434" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="435" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="436" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="437" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="438" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="439" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="440" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="441" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="442" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="443" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="444" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="445" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="446" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="447" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="448" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="449" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="450" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="451" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="452" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="453" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="454" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="455" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="456" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="457" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="458" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="459" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="460" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="461" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="462" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="463" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="464" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="465" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="466" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="467" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="468" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="469" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="470" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="471" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="472" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="473" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="474" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="475" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="476" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="477" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="478" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="479" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="480" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="481" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="482" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="483" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="484" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="485" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="486" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="487" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="488" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="489" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="490" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="491" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="492" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="493" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="494" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="495" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="496" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="497" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="498" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="499" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="500" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="501" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="502" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="503" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="504" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="505" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="506" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="507" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="508" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="509" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="510" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="511" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="512" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="513" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="514" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="515" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="516" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="517" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="518" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="519" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="520" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="521" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="522" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="523" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="524" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="525" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="526" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="527" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="528" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="529" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="530" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="531" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="532" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="533" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="534" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="535" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="536" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="537" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="538" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="539" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="540" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="541" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="542" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="543" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="544" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="545" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="546" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="547" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="548" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="549" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="550" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="551" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="552" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="553" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="554" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="555" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="556" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="557" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="558" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="559" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="560" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="561" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="562" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="563" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="564" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="565" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="566" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="567" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="568" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="569" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="570" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="571" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="572" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="573" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="574" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="575" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="576" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="577" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="578" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="579" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="580" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="581" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="582" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="583" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="584" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="585" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="586" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="587" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="588" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="589" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="590" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="591" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="592" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="593" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="594" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="595" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="596" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="597" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="598" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="599" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="600" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="601" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="602" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="603" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="604" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="605" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="606" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="607" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="608" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="609" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="610" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="611" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="612" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="613" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="614" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="615" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="616" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="617" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="618" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="619" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="620" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="621" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="622" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="623" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="624" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="625" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="626" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="627" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="628" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="629" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="630" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="631" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="632" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="633" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="634" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="635" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="636" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="637" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="638" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="639" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="640" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="641" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="642" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="643" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="644" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="645" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="646" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="647" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="648" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="649" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="650" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="651" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="652" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="653" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="654" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="655" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="656" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="657" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="658" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="659" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="660" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="661" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="662" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="663" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="664" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="665" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="666" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="667" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="668" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="669" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="670" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="671" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="672" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="673" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="674" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="675" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="676" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="677" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="678" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="679" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="680" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="681" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="682" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="683" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="684" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="685" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="686" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="687" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="688" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="689" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="690" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="691" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="692" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="693" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="694" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="695" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="696" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="697" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="698" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="699" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="700" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="701" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="702" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="703" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="704" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="705" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="706" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="707" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="708" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="709" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="710" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="711" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="712" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="713" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="714" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="715" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="716" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="717" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="718" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="719" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="720" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="721" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="722" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="723" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="724" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="725" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="726" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="727" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="728" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="729" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="730" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="731" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="732" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="733" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="734" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="735" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="736" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="737" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="738" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="739" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="740" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="741" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="742" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="743" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="744" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="745" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="746" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="747" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="748" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="749" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="750" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="751" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="752" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="753" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="754" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="755" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="756" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="757" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="758" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="759" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="760" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="761" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="762" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="763" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="764" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="765" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="766" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="767" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="768" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="769" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="770" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="771" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="772" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="773" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="774" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="775" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="776" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="777" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="778" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="779" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="780" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="781" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="782" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="783" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="784" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="785" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="786" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="787" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="788" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="789" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="790" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="791" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="792" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="793" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="794" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="795" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="796" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="797" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="798" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="799" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="800" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="801" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="802" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="803" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="804" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="805" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="806" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="807" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="808" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="809" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="810" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="811" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="812" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="813" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="814" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="815" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="816" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="817" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="818" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="819" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="820" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="821" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="822" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="823" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="824" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="825" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="826" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="827" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="828" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="829" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="830" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="831" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="832" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="833" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="834" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="835" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="836" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="837" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="838" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="839" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="840" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="841" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="842" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="843" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="844" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="845" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="846" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="847" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="848" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="849" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="850" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="851" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="852" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="853" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="854" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="855" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="856" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="857" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="858" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="859" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="860" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="861" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="862" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="863" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="864" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="865" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="866" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="867" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="868" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="869" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="870" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="871" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="872" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="873" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="874" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="875" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="876" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="877" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="878" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="879" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="880" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="881" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="882" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="883" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="884" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="885" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="886" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="887" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="888" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="889" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="890" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="891" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="892" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="893" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="894" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="895" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="896" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="897" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="898" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="899" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="900" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="901" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="902" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="903" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="904" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="905" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="906" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="907" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="908" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="909" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="910" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="911" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="912" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="913" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="914" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="915" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="916" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="917" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="918" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="919" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="920" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="921" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="922" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="923" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="924" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="925" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="926" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="927" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="928" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="929" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="930" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="931" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="932" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="933" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="934" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="935" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="936" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="937" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="938" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="939" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="940" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="941" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="942" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="943" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="944" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="945" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="946" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="947" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="948" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="949" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="950" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="951" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="952" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="953" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="954" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="955" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="956" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="957" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="958" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="959" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="960" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="961" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="962" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="963" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="964" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="965" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="966" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="967" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="968" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="969" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="970" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="971" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="972" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="973" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="974" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="975" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="976" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="977" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="978" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="979" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="980" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="981" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="982" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="983" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="984" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="985" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="986" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="987" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="988" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="989" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="990" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="991" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="992" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="993" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="994" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="995" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="996" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="997" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="998" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="999" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1000" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1001" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1002" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1003" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1004" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1005" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1006" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1007" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1008" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1009" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1010" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1011" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1012" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1013" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1014" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1015" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1016" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1017" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1018" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1019" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1020" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1021" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1022" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1023" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1024" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1025" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1026" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1027" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1028" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1029" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1030" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1031" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1032" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1033" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1034" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1035" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1036" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1037" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1038" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1039" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1040" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1041" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1042" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1043" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1044" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1045" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1046" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1047" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1049" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1050" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1051" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1052" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="E85" s="0"/>
+    </row>
+    <row r="86" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B86" s="0"/>
+      <c r="C86" s="0"/>
+      <c r="D86" s="0"/>
+      <c r="E86" s="0"/>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="H41" r:id="rId1" display="https://arxiv.org/abs/1509.06264"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -4548,113 +3714,113 @@
   </sheetPr>
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1683673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.2908163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.8571428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.2551020408163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.4591836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.3214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>184</v>
+        <v>228</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>185</v>
+        <v>229</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>186</v>
+        <v>230</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>187</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>188</v>
+        <v>232</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>189</v>
+        <v>233</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>190</v>
+        <v>234</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>191</v>
+        <v>235</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>192</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="0" t="s">
-        <v>193</v>
+        <v>237</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>193</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>194</v>
+        <v>238</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>195</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>196</v>
+        <v>240</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>197</v>
+        <v>241</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
-        <v>198</v>
+        <v>242</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>199</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>200</v>
+        <v>244</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>201</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>202</v>
+        <v>246</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>202</v>
+        <v>246</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>203</v>
+        <v>247</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>204</v>
+        <v>248</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>205</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed <Source>._x_pix to .x_pix
</commit_message>
<xml_diff>
--- a/SimCADO/simcado/docs/SimCADO_defaults.xlsx
+++ b/SimCADO/simcado/docs/SimCADO_defaults.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -991,29 +991,29 @@
   </sheetPr>
   <dimension ref="A1:Z88"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E44" activeCellId="0" sqref="E44"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.25"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="31.7244897959184"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="30.780612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="45.6275510204082"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="14" min="12" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="31.3163265306122"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="30.3724489795918"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="173.382653061224"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="59.8928571428572"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="40.7959183673469"/>
+    <col collapsed="false" hidden="false" max="14" min="12" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="1" width="12.9591836734694"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1071,7 +1071,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="159.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="83.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -1105,7 +1105,7 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="67.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="69.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
@@ -1149,7 +1149,7 @@
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
     </row>
-    <row r="4" customFormat="false" ht="290.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="110.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>26</v>
@@ -1181,7 +1181,7 @@
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
     </row>
-    <row r="5" customFormat="false" ht="67.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="27.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -1223,7 +1223,7 @@
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="67.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="27.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2"/>
       <c r="B6" s="0"/>
       <c r="C6" s="2" t="s">
@@ -1265,7 +1265,7 @@
       <c r="Y6" s="2"/>
       <c r="Z6" s="2"/>
     </row>
-    <row r="7" customFormat="false" ht="54.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="27.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
@@ -1309,7 +1309,7 @@
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
     </row>
-    <row r="8" customFormat="false" ht="159.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="83.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>43</v>
@@ -1341,7 +1341,7 @@
       <c r="Y8" s="2"/>
       <c r="Z8" s="2"/>
     </row>
-    <row r="9" customFormat="false" ht="54.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="27.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
@@ -1383,7 +1383,7 @@
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
     </row>
-    <row r="10" customFormat="false" ht="41.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="41.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
@@ -1425,7 +1425,7 @@
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
     </row>
-    <row r="11" customFormat="false" ht="106.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="41.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>52</v>
       </c>
@@ -1459,7 +1459,7 @@
       <c r="Y11" s="2"/>
       <c r="Z11" s="2"/>
     </row>
-    <row r="12" customFormat="false" ht="41.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="41.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
@@ -1499,7 +1499,7 @@
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
     </row>
-    <row r="13" customFormat="false" ht="41.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="41.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
@@ -1543,7 +1543,7 @@
       <c r="Y13" s="2"/>
       <c r="Z13" s="2"/>
     </row>
-    <row r="14" customFormat="false" ht="264.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="207.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
         <v>63</v>
@@ -1575,7 +1575,7 @@
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
     </row>
-    <row r="15" customFormat="false" ht="77.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="83.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
@@ -1619,7 +1619,7 @@
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
     </row>
-    <row r="16" customFormat="false" ht="41.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
         <v>69</v>
@@ -1651,7 +1651,7 @@
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
     </row>
-    <row r="17" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="41.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
@@ -1693,7 +1693,7 @@
       <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
     </row>
-    <row r="18" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="41.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
@@ -1737,7 +1737,7 @@
       <c r="Y18" s="2"/>
       <c r="Z18" s="2"/>
     </row>
-    <row r="19" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="27.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
         <v>78</v>
@@ -1769,7 +1769,7 @@
       <c r="Y19" s="2"/>
       <c r="Z19" s="2"/>
     </row>
-    <row r="20" customFormat="false" ht="77.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="41.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
@@ -1811,7 +1811,7 @@
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
     </row>
-    <row r="21" customFormat="false" ht="146.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="69.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
         <v>85</v>
@@ -1843,7 +1843,7 @@
       <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>
     </row>
-    <row r="22" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="55.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
@@ -1887,7 +1887,7 @@
       <c r="Y22" s="2"/>
       <c r="Z22" s="2"/>
     </row>
-    <row r="23" customFormat="false" ht="67.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="41.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
         <v>91</v>
@@ -1919,7 +1919,7 @@
       <c r="Y23" s="2"/>
       <c r="Z23" s="2"/>
     </row>
-    <row r="24" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="41.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
@@ -1961,7 +1961,7 @@
       <c r="Y24" s="2"/>
       <c r="Z24" s="2"/>
     </row>
-    <row r="25" customFormat="false" ht="54.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="27.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -2003,7 +2003,7 @@
       <c r="Y25" s="2"/>
       <c r="Z25" s="2"/>
     </row>
-    <row r="26" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
         <v>98</v>
@@ -2035,7 +2035,7 @@
       <c r="Y26" s="2"/>
       <c r="Z26" s="2"/>
     </row>
-    <row r="27" customFormat="false" ht="41.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="41.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
@@ -2077,7 +2077,7 @@
       <c r="Y27" s="2"/>
       <c r="Z27" s="2"/>
     </row>
-    <row r="28" customFormat="false" ht="41.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="27.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
@@ -2119,7 +2119,7 @@
       <c r="Y28" s="2"/>
       <c r="Z28" s="2"/>
     </row>
-    <row r="29" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="27.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
         <v>106</v>
       </c>
@@ -2151,7 +2151,7 @@
       <c r="Y29" s="2"/>
       <c r="Z29" s="2"/>
     </row>
-    <row r="30" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="27.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2"/>
       <c r="B30" s="0"/>
       <c r="C30" s="2" t="s">
@@ -2193,7 +2193,7 @@
       <c r="Y30" s="2"/>
       <c r="Z30" s="2"/>
     </row>
-    <row r="31" customFormat="false" ht="159.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="83.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2"/>
       <c r="B31" s="1" t="s">
         <v>114</v>
@@ -2225,7 +2225,7 @@
       <c r="Y31" s="2"/>
       <c r="Z31" s="2"/>
     </row>
-    <row r="32" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2"/>
       <c r="B32" s="0"/>
       <c r="C32" s="2" t="s">
@@ -2261,7 +2261,7 @@
       <c r="Y32" s="2"/>
       <c r="Z32" s="2"/>
     </row>
-    <row r="33" customFormat="false" ht="67.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="69.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2"/>
       <c r="B33" s="0"/>
       <c r="C33" s="2" t="s">
@@ -2299,7 +2299,7 @@
       <c r="Y33" s="2"/>
       <c r="Z33" s="2"/>
     </row>
-    <row r="34" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2"/>
       <c r="B34" s="0"/>
       <c r="C34" s="2" t="s">
@@ -2335,7 +2335,7 @@
       <c r="Y34" s="2"/>
       <c r="Z34" s="2"/>
     </row>
-    <row r="35" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2"/>
       <c r="B35" s="0"/>
       <c r="C35" s="2" t="s">
@@ -2371,7 +2371,7 @@
       <c r="Y35" s="2"/>
       <c r="Z35" s="2"/>
     </row>
-    <row r="36" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2"/>
       <c r="B36" s="0"/>
       <c r="C36" s="2" t="s">
@@ -2407,7 +2407,7 @@
       <c r="Y36" s="2"/>
       <c r="Z36" s="2"/>
     </row>
-    <row r="37" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2"/>
       <c r="B37" s="0"/>
       <c r="C37" s="2" t="s">
@@ -2473,7 +2473,7 @@
       <c r="Y38" s="2"/>
       <c r="Z38" s="2"/>
     </row>
-    <row r="39" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="27.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2"/>
       <c r="B39" s="0"/>
       <c r="C39" s="2"/>
@@ -2507,7 +2507,7 @@
       <c r="Y39" s="2"/>
       <c r="Z39" s="2"/>
     </row>
-    <row r="40" customFormat="false" ht="41.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="41.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2"/>
       <c r="B40" s="0"/>
       <c r="C40" s="2"/>
@@ -2541,7 +2541,7 @@
       <c r="Y40" s="2"/>
       <c r="Z40" s="2"/>
     </row>
-    <row r="41" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="27.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2"/>
       <c r="B41" s="0"/>
       <c r="C41" s="2"/>
@@ -2605,7 +2605,7 @@
       <c r="Y42" s="2"/>
       <c r="Z42" s="2"/>
     </row>
-    <row r="43" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0"/>
       <c r="B43" s="4" t="s">
         <v>138</v>
@@ -2637,7 +2637,7 @@
       <c r="Y43" s="2"/>
       <c r="Z43" s="2"/>
     </row>
-    <row r="44" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0"/>
       <c r="B44" s="4"/>
       <c r="C44" s="2" t="s">
@@ -2673,7 +2673,7 @@
       <c r="Y44" s="2"/>
       <c r="Z44" s="2"/>
     </row>
-    <row r="45" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0"/>
       <c r="B45" s="4"/>
       <c r="C45" s="2" t="s">
@@ -2709,7 +2709,7 @@
       <c r="Y45" s="2"/>
       <c r="Z45" s="2"/>
     </row>
-    <row r="46" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0"/>
       <c r="B46" s="4"/>
       <c r="C46" s="2" t="s">
@@ -2745,7 +2745,7 @@
       <c r="Y46" s="2"/>
       <c r="Z46" s="2"/>
     </row>
-    <row r="47" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0"/>
       <c r="B47" s="4"/>
       <c r="C47" s="2" t="s">
@@ -2781,7 +2781,7 @@
       <c r="Y47" s="2"/>
       <c r="Z47" s="2"/>
     </row>
-    <row r="48" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0"/>
       <c r="B48" s="0"/>
       <c r="C48" s="2" t="s">
@@ -2817,7 +2817,7 @@
       <c r="Y48" s="2"/>
       <c r="Z48" s="2"/>
     </row>
-    <row r="49" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0"/>
       <c r="B49" s="0"/>
       <c r="C49" s="2" t="s">
@@ -2853,7 +2853,7 @@
       <c r="Y49" s="2"/>
       <c r="Z49" s="2"/>
     </row>
-    <row r="50" customFormat="false" ht="133.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="83.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0"/>
       <c r="B50" s="1" t="s">
         <v>154</v>
@@ -2885,7 +2885,7 @@
       <c r="Y50" s="2"/>
       <c r="Z50" s="2"/>
     </row>
-    <row r="51" customFormat="false" ht="41.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="41.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0"/>
       <c r="B51" s="0"/>
       <c r="C51" s="2" t="s">
@@ -2921,7 +2921,7 @@
       <c r="Y51" s="2"/>
       <c r="Z51" s="2"/>
     </row>
-    <row r="52" customFormat="false" ht="67.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="69.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0"/>
       <c r="B52" s="0"/>
       <c r="C52" s="2" t="s">
@@ -2961,7 +2961,7 @@
       <c r="Y52" s="2"/>
       <c r="Z52" s="2"/>
     </row>
-    <row r="53" customFormat="false" ht="67.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="69.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0"/>
       <c r="B53" s="0"/>
       <c r="C53" s="2" t="s">
@@ -2997,7 +2997,7 @@
       <c r="Y53" s="2"/>
       <c r="Z53" s="2"/>
     </row>
-    <row r="54" customFormat="false" ht="316.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="193.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0"/>
       <c r="B54" s="1" t="s">
         <v>164</v>
@@ -3029,7 +3029,7 @@
       <c r="Y54" s="2"/>
       <c r="Z54" s="2"/>
     </row>
-    <row r="55" customFormat="false" ht="80.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="83.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0"/>
       <c r="B55" s="0"/>
       <c r="C55" s="2" t="s">
@@ -3065,7 +3065,7 @@
       <c r="Y55" s="2"/>
       <c r="Z55" s="2"/>
     </row>
-    <row r="56" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="27.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2"/>
       <c r="B56" s="2" t="s">
         <v>169</v>
@@ -3123,7 +3123,7 @@
       <c r="Y57" s="2"/>
       <c r="Z57" s="2"/>
     </row>
-    <row r="58" customFormat="false" ht="119.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="55.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
         <v>170</v>
       </c>
@@ -3157,7 +3157,7 @@
       <c r="Y58" s="2"/>
       <c r="Z58" s="2"/>
     </row>
-    <row r="59" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2" t="s">
@@ -3191,7 +3191,7 @@
       <c r="Y59" s="2"/>
       <c r="Z59" s="2"/>
     </row>
-    <row r="60" customFormat="false" ht="67.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="69.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2" t="s">
@@ -3233,7 +3233,7 @@
       <c r="Y60" s="2"/>
       <c r="Z60" s="2"/>
     </row>
-    <row r="61" customFormat="false" ht="41.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="41.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2" t="s">
@@ -3277,7 +3277,7 @@
       <c r="Y61" s="2"/>
       <c r="Z61" s="2"/>
     </row>
-    <row r="62" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="27.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2" t="s">
@@ -3317,7 +3317,7 @@
       <c r="Y62" s="2"/>
       <c r="Z62" s="2"/>
     </row>
-    <row r="63" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="27.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2" t="s">
@@ -3355,7 +3355,7 @@
       <c r="Y63" s="2"/>
       <c r="Z63" s="2"/>
     </row>
-    <row r="64" customFormat="false" ht="106.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="41.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
         <v>186</v>
       </c>
@@ -3389,7 +3389,7 @@
       <c r="Y64" s="2"/>
       <c r="Z64" s="2"/>
     </row>
-    <row r="65" customFormat="false" ht="41.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="41.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0"/>
       <c r="B65" s="0"/>
       <c r="C65" s="1" t="s">
@@ -3431,7 +3431,7 @@
       <c r="Y65" s="2"/>
       <c r="Z65" s="2"/>
     </row>
-    <row r="66" customFormat="false" ht="41.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="41.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0"/>
       <c r="B66" s="0"/>
       <c r="C66" s="1" t="s">
@@ -3469,7 +3469,7 @@
       <c r="Y66" s="2"/>
       <c r="Z66" s="2"/>
     </row>
-    <row r="67" customFormat="false" ht="41.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="41.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0"/>
       <c r="B67" s="0"/>
       <c r="C67" s="1" t="s">
@@ -3509,7 +3509,7 @@
       <c r="Y67" s="2"/>
       <c r="Z67" s="2"/>
     </row>
-    <row r="68" customFormat="false" ht="41.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="41.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2"/>
       <c r="B68" s="2" t="s">
         <v>198</v>
@@ -3522,8 +3522,9 @@
       <c r="H68" s="0"/>
       <c r="I68" s="0"/>
       <c r="J68" s="0"/>
-    </row>
-    <row r="69" customFormat="false" ht="41.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K68" s="0"/>
+    </row>
+    <row r="69" customFormat="false" ht="41.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0"/>
       <c r="B69" s="0"/>
       <c r="C69" s="1" t="s">
@@ -3544,7 +3545,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="41.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="41.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0"/>
       <c r="B70" s="0"/>
       <c r="C70" s="1" t="s">
@@ -3558,12 +3559,13 @@
       </c>
       <c r="F70" s="0"/>
       <c r="G70" s="0"/>
+      <c r="H70" s="0"/>
       <c r="J70" s="0"/>
       <c r="K70" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="93.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="110.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0"/>
       <c r="B71" s="0"/>
       <c r="C71" s="1" t="s">
@@ -3575,12 +3577,15 @@
       <c r="E71" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="F71" s="0"/>
+      <c r="G71" s="0"/>
+      <c r="H71" s="0"/>
       <c r="J71" s="0"/>
       <c r="K71" s="1" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
         <v>206</v>
       </c>
@@ -3590,9 +3595,13 @@
       <c r="C72" s="0"/>
       <c r="D72" s="0"/>
       <c r="E72" s="0"/>
+      <c r="F72" s="0"/>
+      <c r="G72" s="0"/>
+      <c r="H72" s="0"/>
       <c r="J72" s="0"/>
-    </row>
-    <row r="73" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K72" s="0"/>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2"/>
       <c r="B73" s="0"/>
       <c r="C73" s="2" t="s">
@@ -3604,12 +3613,15 @@
       <c r="E73" s="1" t="s">
         <v>117</v>
       </c>
+      <c r="F73" s="0"/>
+      <c r="G73" s="0"/>
+      <c r="H73" s="0"/>
       <c r="J73" s="0"/>
       <c r="K73" s="1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="54.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="55.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0"/>
       <c r="B74" s="0"/>
       <c r="C74" s="0"/>
@@ -3625,6 +3637,7 @@
       <c r="G74" s="8" t="n">
         <v>42370</v>
       </c>
+      <c r="H74" s="0"/>
       <c r="J74" s="1" t="s">
         <v>214</v>
       </c>
@@ -3632,7 +3645,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0"/>
       <c r="B75" s="0"/>
       <c r="C75" s="0"/>
@@ -3642,12 +3655,15 @@
       <c r="E75" s="1" t="s">
         <v>217</v>
       </c>
+      <c r="F75" s="0"/>
+      <c r="G75" s="0"/>
+      <c r="H75" s="0"/>
       <c r="J75" s="0"/>
       <c r="K75" s="0" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0"/>
       <c r="B76" s="2" t="s">
         <v>219</v>
@@ -3655,9 +3671,13 @@
       <c r="C76" s="0"/>
       <c r="D76" s="0"/>
       <c r="E76" s="0"/>
+      <c r="F76" s="0"/>
+      <c r="G76" s="0"/>
+      <c r="H76" s="0"/>
       <c r="J76" s="0"/>
-    </row>
-    <row r="77" customFormat="false" ht="41.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K76" s="0"/>
+    </row>
+    <row r="77" customFormat="false" ht="55.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0"/>
       <c r="B77" s="0"/>
       <c r="C77" s="2" t="s">
@@ -3675,6 +3695,7 @@
       <c r="G77" s="8" t="n">
         <v>42370</v>
       </c>
+      <c r="H77" s="0"/>
       <c r="J77" s="1" t="s">
         <v>221</v>
       </c>
@@ -3682,7 +3703,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="27.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2"/>
       <c r="B78" s="2" t="s">
         <v>223</v>
@@ -3690,8 +3711,12 @@
       <c r="C78" s="0"/>
       <c r="D78" s="0"/>
       <c r="E78" s="0"/>
-    </row>
-    <row r="79" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F78" s="0"/>
+      <c r="G78" s="0"/>
+      <c r="H78" s="0"/>
+      <c r="K78" s="0"/>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2" t="s">
@@ -3703,11 +3728,14 @@
       <c r="E79" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="F79" s="0"/>
+      <c r="G79" s="0"/>
+      <c r="H79" s="0"/>
       <c r="K79" s="1" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0"/>
       <c r="B80" s="0"/>
       <c r="C80" s="2"/>
@@ -3717,11 +3745,14 @@
       <c r="E80" s="1" t="n">
         <v>750</v>
       </c>
+      <c r="F80" s="0"/>
+      <c r="G80" s="0"/>
+      <c r="H80" s="0"/>
       <c r="K80" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0"/>
       <c r="B81" s="0"/>
       <c r="C81" s="0"/>
@@ -3731,11 +3762,14 @@
       <c r="E81" s="9" t="s">
         <v>229</v>
       </c>
+      <c r="F81" s="0"/>
+      <c r="G81" s="0"/>
+      <c r="H81" s="0"/>
       <c r="K81" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="27.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0"/>
       <c r="B82" s="1" t="s">
         <v>231</v>
@@ -3743,11 +3777,14 @@
       <c r="C82" s="0"/>
       <c r="D82" s="0"/>
       <c r="E82" s="0"/>
+      <c r="F82" s="0"/>
+      <c r="G82" s="0"/>
       <c r="H82" s="1" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="83" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K82" s="0"/>
+    </row>
+    <row r="83" customFormat="false" ht="27.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0"/>
       <c r="B83" s="0"/>
       <c r="C83" s="1" t="s">
@@ -3769,7 +3806,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0"/>
       <c r="B84" s="0"/>
       <c r="C84" s="1" t="s">
@@ -3791,7 +3828,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0"/>
       <c r="B85" s="0"/>
       <c r="C85" s="1" t="s">
@@ -3827,7 +3864,7 @@
       <c r="D87" s="0"/>
       <c r="E87" s="0"/>
     </row>
-    <row r="88" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="s">
         <v>241</v>
       </c>
@@ -3854,21 +3891,20 @@
   </sheetPr>
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>